<commit_message>
Update to include User Types associated with the Products
</commit_message>
<xml_diff>
--- a/data/BusinessCapabilitiesv0.1.xlsx
+++ b/data/BusinessCapabilitiesv0.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leegath/LAG/Fathomatics/code/nhse/capabilitygenerator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E583BA3-D7FA-6348-B2AB-F9FE83E3220C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA1B443-1E9B-C944-8F26-E94A411EEB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34120" yWindow="500" windowWidth="34140" windowHeight="26580" activeTab="3" xr2:uid="{FB9E69F6-520F-B448-8326-5E7FF50D6D4B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="26580" activeTab="3" xr2:uid="{FB9E69F6-520F-B448-8326-5E7FF50D6D4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Capability Map" sheetId="10" r:id="rId1"/>
@@ -404,7 +404,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1485" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="459">
   <si>
     <t>Value Stream Stage</t>
   </si>
@@ -2514,12 +2514,30 @@
   <si>
     <t>5.2 Support Research</t>
   </si>
+  <si>
+    <t>Participant, Clinical Staff, Operational Staff</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>Operational Staff</t>
+  </si>
+  <si>
+    <t>System User</t>
+  </si>
+  <si>
+    <t>Participant, Operational Staff</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2579,6 +2597,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="30">
@@ -3098,7 +3123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="337">
+  <cellXfs count="339">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4034,6 +4059,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -23531,9 +23558,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771BD26-5CB2-F242-A0FA-A4D8589272A0}">
   <dimension ref="A1:BO73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D63" sqref="D63"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23547,6 +23574,7 @@
     <col min="8" max="8" width="52.6640625" style="175" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" style="128" customWidth="1"/>
     <col min="10" max="10" width="97" customWidth="1"/>
+    <col min="11" max="11" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" s="1" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -23580,7 +23608,9 @@
       <c r="J1" s="114" t="s">
         <v>443</v>
       </c>
-      <c r="K1" s="117"/>
+      <c r="K1" s="338" t="s">
+        <v>458</v>
+      </c>
       <c r="L1" s="114"/>
       <c r="M1" s="114"/>
       <c r="N1" s="114"/>
@@ -23638,7 +23668,7 @@
       <c r="BN1" s="114"/>
       <c r="BO1" s="114"/>
     </row>
-    <row r="2" spans="1:67" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" s="1" customFormat="1" ht="204" x14ac:dyDescent="0.2">
       <c r="A2" s="108" t="s">
         <v>7</v>
       </c>
@@ -23670,7 +23700,10 @@
         <f>VLOOKUP(I2,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K2" s="114"/>
+      <c r="K2" s="126" t="str">
+        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L2" s="114"/>
       <c r="M2" s="114"/>
       <c r="N2" s="114"/>
@@ -23760,7 +23793,10 @@
         <f>VLOOKUP(I3,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K3" s="114"/>
+      <c r="K3" s="126" t="str">
+        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L3" s="114"/>
       <c r="M3" s="114"/>
       <c r="N3" s="114"/>
@@ -23850,7 +23886,10 @@
         <f>VLOOKUP(I4,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K4" s="114"/>
+      <c r="K4" s="126" t="str">
+        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L4" s="114"/>
       <c r="M4" s="114"/>
       <c r="N4" s="114"/>
@@ -23940,7 +23979,10 @@
         <f>VLOOKUP(I5,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K5" s="117"/>
+      <c r="K5" s="126" t="str">
+        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L5" s="117"/>
       <c r="M5" s="117"/>
       <c r="N5" s="117"/>
@@ -24030,7 +24072,10 @@
         <f>VLOOKUP(I6,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K6" s="117"/>
+      <c r="K6" s="126" t="e">
+        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="L6" s="117"/>
       <c r="M6" s="117"/>
       <c r="N6" s="117"/>
@@ -24120,7 +24165,10 @@
         <f>VLOOKUP(I7,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Campaign Manager allows the segmentation of participants according to different characteristics e.g. demographics or clinical risk factors and tailor screening pathway outreach accordingly to maximise uptake. It enables personalisation of health communication campaigns and allows the impact of these campaigns to be assessed.</v>
       </c>
-      <c r="K7" s="117"/>
+      <c r="K7" s="126" t="str">
+        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L7" s="117"/>
       <c r="M7" s="117"/>
       <c r="N7" s="117"/>
@@ -24210,7 +24258,10 @@
         <f>VLOOKUP(I8,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Campaign Manager allows the segmentation of participants according to different characteristics e.g. demographics or clinical risk factors and tailor screening pathway outreach accordingly to maximise uptake. It enables personalisation of health communication campaigns and allows the impact of these campaigns to be assessed.</v>
       </c>
-      <c r="K8" s="117"/>
+      <c r="K8" s="126" t="str">
+        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L8" s="117"/>
       <c r="M8" s="117"/>
       <c r="N8" s="117"/>
@@ -24300,7 +24351,10 @@
         <f>VLOOKUP(I9,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K9" s="117"/>
+      <c r="K9" s="126" t="str">
+        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L9" s="117"/>
       <c r="M9" s="117"/>
       <c r="N9" s="117"/>
@@ -24390,7 +24444,10 @@
         <f>VLOOKUP(I10,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity Manager provides a centralised way of understanding and managing capacity across screening pathways. Providers are able to provide and amend their local capacity, with resulting available 'slots' feeding into the allocation process.</v>
       </c>
-      <c r="K10" s="117"/>
+      <c r="K10" s="126" t="str">
+        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L10" s="117"/>
       <c r="M10" s="117"/>
       <c r="N10" s="117"/>
@@ -24480,7 +24537,10 @@
         <f>VLOOKUP(I11,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
-      <c r="K11" s="117"/>
+      <c r="K11" s="126" t="str">
+        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L11" s="117"/>
       <c r="M11" s="117"/>
       <c r="N11" s="117"/>
@@ -24570,7 +24630,10 @@
         <f>VLOOKUP(I12,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
-      <c r="K12" s="117"/>
+      <c r="K12" s="126" t="str">
+        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L12" s="117"/>
       <c r="M12" s="117"/>
       <c r="N12" s="117"/>
@@ -24660,7 +24723,10 @@
         <f>VLOOKUP(I13,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity Manager provides a centralised way of understanding and managing capacity across screening pathways. Providers are able to provide and amend their local capacity, with resulting available 'slots' feeding into the allocation process.</v>
       </c>
-      <c r="K13" s="117"/>
+      <c r="K13" s="126" t="str">
+        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L13" s="117"/>
       <c r="M13" s="117"/>
       <c r="N13" s="117"/>
@@ -24750,7 +24816,10 @@
         <f>VLOOKUP(I14,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
-      <c r="K14" s="117"/>
+      <c r="K14" s="126" t="str">
+        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L14" s="117"/>
       <c r="M14" s="117"/>
       <c r="N14" s="117"/>
@@ -24840,7 +24909,10 @@
         <f>VLOOKUP(I15,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
-      <c r="K15" s="117"/>
+      <c r="K15" s="126" t="str">
+        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L15" s="117"/>
       <c r="M15" s="117"/>
       <c r="N15" s="117"/>
@@ -24930,7 +25002,10 @@
         <f>VLOOKUP(I16,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
-      <c r="K16" s="117"/>
+      <c r="K16" s="126" t="str">
+        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L16" s="117"/>
       <c r="M16" s="117"/>
       <c r="N16" s="117"/>
@@ -25020,7 +25095,10 @@
         <f>VLOOKUP(I17,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="K17" s="117"/>
+      <c r="K17" s="126" t="e">
+        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="L17" s="117"/>
       <c r="M17" s="117"/>
       <c r="N17" s="117"/>
@@ -25110,7 +25188,10 @@
         <f>VLOOKUP(I18,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K18" s="117"/>
+      <c r="K18" s="126" t="str">
+        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L18" s="117"/>
       <c r="M18" s="117"/>
       <c r="N18" s="117"/>
@@ -25200,7 +25281,10 @@
         <f>VLOOKUP(I19,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
-      <c r="K19" s="117"/>
+      <c r="K19" s="126" t="str">
+        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L19" s="117"/>
       <c r="M19" s="117"/>
       <c r="N19" s="117"/>
@@ -25290,7 +25374,10 @@
         <f>VLOOKUP(I20,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
-      <c r="K20" s="117"/>
+      <c r="K20" s="126" t="str">
+        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L20" s="117"/>
       <c r="M20" s="117"/>
       <c r="N20" s="117"/>
@@ -25380,7 +25467,10 @@
         <f>VLOOKUP(I21,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
-      <c r="K21" s="117"/>
+      <c r="K21" s="126" t="str">
+        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L21" s="117"/>
       <c r="M21" s="117"/>
       <c r="N21" s="117"/>
@@ -25470,7 +25560,10 @@
         <f>VLOOKUP(I22,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
-      <c r="K22" s="117"/>
+      <c r="K22" s="126" t="str">
+        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L22" s="117"/>
       <c r="M22" s="117"/>
       <c r="N22" s="117"/>
@@ -25560,7 +25653,10 @@
         <f>VLOOKUP(I23,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Allocator is a pathway agnostic allocation engine. It provides a set of allocation algorithms and uses participant preferences and needs e.g. accessibility criteria to optimally allocate individuals to 'slots'.</v>
       </c>
-      <c r="K23" s="117"/>
+      <c r="K23" s="126" t="str">
+        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>System User</v>
+      </c>
       <c r="L23" s="117"/>
       <c r="M23" s="117"/>
       <c r="N23" s="117"/>
@@ -25650,7 +25746,10 @@
         <f>VLOOKUP(I24,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Allocator is a pathway agnostic allocation engine. It provides a set of allocation algorithms and uses participant preferences and needs e.g. accessibility criteria to optimally allocate individuals to 'slots'.</v>
       </c>
-      <c r="K24" s="117"/>
+      <c r="K24" s="126" t="str">
+        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>System User</v>
+      </c>
       <c r="L24" s="117"/>
       <c r="M24" s="117"/>
       <c r="N24" s="117"/>
@@ -25740,7 +25839,10 @@
         <f>VLOOKUP(I25,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K25" s="117"/>
+      <c r="K25" s="126" t="str">
+        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L25" s="117"/>
       <c r="M25" s="117"/>
       <c r="N25" s="117"/>
@@ -25830,7 +25932,10 @@
         <f>VLOOKUP(I26,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K26" s="117"/>
+      <c r="K26" s="126" t="str">
+        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L26" s="117"/>
       <c r="M26" s="117"/>
       <c r="N26" s="117"/>
@@ -25920,7 +26025,10 @@
         <f>VLOOKUP(I27,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K27" s="117"/>
+      <c r="K27" s="126" t="str">
+        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L27" s="117"/>
       <c r="M27" s="117"/>
       <c r="N27" s="117"/>
@@ -26010,7 +26118,10 @@
         <f>VLOOKUP(I28,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K28" s="117"/>
+      <c r="K28" s="126" t="str">
+        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L28" s="117"/>
       <c r="M28" s="117"/>
       <c r="N28" s="117"/>
@@ -26100,7 +26211,10 @@
         <f>VLOOKUP(I29,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
-      <c r="K29" s="117"/>
+      <c r="K29" s="126" t="str">
+        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L29" s="117"/>
       <c r="M29" s="117"/>
       <c r="N29" s="117"/>
@@ -26190,7 +26304,10 @@
         <f>VLOOKUP(I30,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K30" s="117"/>
+      <c r="K30" s="126" t="str">
+        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L30" s="117"/>
       <c r="M30" s="117"/>
       <c r="N30" s="117"/>
@@ -26280,7 +26397,10 @@
         <f>VLOOKUP(I31,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K31" s="117"/>
+      <c r="K31" s="126" t="str">
+        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L31" s="117"/>
       <c r="M31" s="117"/>
       <c r="N31" s="117"/>
@@ -26370,7 +26490,10 @@
         <f>VLOOKUP(I32,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K32" s="117"/>
+      <c r="K32" s="126" t="str">
+        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L32" s="117"/>
       <c r="M32" s="117"/>
       <c r="N32" s="117"/>
@@ -26460,7 +26583,10 @@
         <f>VLOOKUP(I33,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K33" s="117"/>
+      <c r="K33" s="126" t="str">
+        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L33" s="117"/>
       <c r="M33" s="117"/>
       <c r="N33" s="117"/>
@@ -26550,7 +26676,10 @@
         <f>VLOOKUP(I34,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
-      <c r="K34" s="117"/>
+      <c r="K34" s="126" t="str">
+        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L34" s="117"/>
       <c r="M34" s="117"/>
       <c r="N34" s="117"/>
@@ -26640,7 +26769,10 @@
         <f>VLOOKUP(I35,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
-      <c r="K35" s="117"/>
+      <c r="K35" s="126" t="str">
+        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L35" s="117"/>
       <c r="M35" s="117"/>
       <c r="N35" s="117"/>
@@ -26730,7 +26862,10 @@
         <f>VLOOKUP(I36,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K36" s="117"/>
+      <c r="K36" s="126" t="str">
+        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L36" s="117"/>
       <c r="M36" s="117"/>
       <c r="N36" s="117"/>
@@ -26820,7 +26955,10 @@
         <f>VLOOKUP(I37,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K37" s="117"/>
+      <c r="K37" s="126" t="str">
+        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L37" s="117"/>
       <c r="M37" s="117"/>
       <c r="N37" s="117"/>
@@ -26910,7 +27048,10 @@
         <f>VLOOKUP(I38,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K38" s="117"/>
+      <c r="K38" s="126" t="str">
+        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L38" s="117"/>
       <c r="M38" s="117"/>
       <c r="N38" s="117"/>
@@ -27000,7 +27141,10 @@
         <f>VLOOKUP(I39,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Support allows the efficient handling of inbound queries from participants about the screening pathway and will primarily be used by participant support staff e.g. call centre staff.</v>
       </c>
-      <c r="K39" s="117"/>
+      <c r="K39" s="126" t="str">
+        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L39" s="117"/>
       <c r="M39" s="117"/>
       <c r="N39" s="117"/>
@@ -27090,7 +27234,10 @@
         <f>VLOOKUP(I40,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Support allows the efficient handling of inbound queries from participants about the screening pathway and will primarily be used by participant support staff e.g. call centre staff.</v>
       </c>
-      <c r="K40" s="117"/>
+      <c r="K40" s="126" t="str">
+        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L40" s="117"/>
       <c r="M40" s="117"/>
       <c r="N40" s="117"/>
@@ -27180,7 +27327,10 @@
         <f>VLOOKUP(I41,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K41" s="117"/>
+      <c r="K41" s="126" t="str">
+        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L41" s="117"/>
       <c r="M41" s="117"/>
       <c r="N41" s="117"/>
@@ -27270,7 +27420,10 @@
         <f>VLOOKUP(I42,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
-      <c r="K42" s="117"/>
+      <c r="K42" s="126" t="str">
+        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L42" s="117"/>
       <c r="M42" s="117"/>
       <c r="N42" s="117"/>
@@ -27360,7 +27513,10 @@
         <f>VLOOKUP(I43,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K43" s="117"/>
+      <c r="K43" s="126" t="str">
+        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L43" s="117"/>
       <c r="M43" s="117"/>
       <c r="N43" s="117"/>
@@ -27450,7 +27606,10 @@
         <f>VLOOKUP(I44,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K44" s="117"/>
+      <c r="K44" s="126" t="str">
+        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L44" s="117"/>
       <c r="M44" s="117"/>
       <c r="N44" s="117"/>
@@ -27540,7 +27699,10 @@
         <f>VLOOKUP(I45,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
-      <c r="K45" s="117"/>
+      <c r="K45" s="126" t="str">
+        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L45" s="117"/>
       <c r="M45" s="117"/>
       <c r="N45" s="117"/>
@@ -27630,7 +27792,10 @@
         <f>VLOOKUP(I46,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K46" s="117"/>
+      <c r="K46" s="126" t="str">
+        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L46" s="117"/>
       <c r="M46" s="117"/>
       <c r="N46" s="117"/>
@@ -27720,7 +27885,10 @@
         <f>VLOOKUP(I47,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K47" s="117"/>
+      <c r="K47" s="126" t="str">
+        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L47" s="117"/>
       <c r="M47" s="117"/>
       <c r="N47" s="117"/>
@@ -27810,7 +27978,10 @@
         <f>VLOOKUP(I48,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K48" s="117"/>
+      <c r="K48" s="126" t="str">
+        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L48" s="117"/>
       <c r="M48" s="117"/>
       <c r="N48" s="117"/>
@@ -27900,7 +28071,10 @@
         <f>VLOOKUP(I49,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K49" s="117"/>
+      <c r="K49" s="126" t="str">
+        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L49" s="117"/>
       <c r="M49" s="117"/>
       <c r="N49" s="117"/>
@@ -27990,7 +28164,10 @@
         <f>VLOOKUP(I50,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K50" s="117"/>
+      <c r="K50" s="126" t="str">
+        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L50" s="117"/>
       <c r="M50" s="117"/>
       <c r="N50" s="117"/>
@@ -28080,7 +28257,10 @@
         <f>VLOOKUP(I51,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K51" s="117"/>
+      <c r="K51" s="126" t="str">
+        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L51" s="117"/>
       <c r="M51" s="117"/>
       <c r="N51" s="117"/>
@@ -28170,7 +28350,10 @@
         <f>VLOOKUP(I52,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
-      <c r="K52" s="117"/>
+      <c r="K52" s="126" t="str">
+        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Clinical Staff, Operational Staff</v>
+      </c>
       <c r="L52" s="117"/>
       <c r="M52" s="117"/>
       <c r="N52" s="117"/>
@@ -28260,7 +28443,10 @@
         <f>VLOOKUP(I53,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K53" s="117"/>
+      <c r="K53" s="126" t="str">
+        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L53" s="117"/>
       <c r="M53" s="117"/>
       <c r="N53" s="117"/>
@@ -28350,7 +28536,10 @@
         <f>VLOOKUP(I54,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K54" s="117"/>
+      <c r="K54" s="126" t="str">
+        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L54" s="117"/>
       <c r="M54" s="117"/>
       <c r="N54" s="117"/>
@@ -28440,7 +28629,10 @@
         <f>VLOOKUP(I55,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K55" s="117"/>
+      <c r="K55" s="126" t="str">
+        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L55" s="117"/>
       <c r="M55" s="117"/>
       <c r="N55" s="117"/>
@@ -28530,7 +28722,10 @@
         <f>VLOOKUP(I56,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K56" s="117"/>
+      <c r="K56" s="126" t="str">
+        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L56" s="117"/>
       <c r="M56" s="117"/>
       <c r="N56" s="117"/>
@@ -28620,7 +28815,10 @@
         <f>VLOOKUP(I57,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
-      <c r="K57" s="117"/>
+      <c r="K57" s="126" t="str">
+        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Participant, Operational Staff</v>
+      </c>
       <c r="L57" s="117"/>
       <c r="M57" s="117"/>
       <c r="N57" s="117"/>
@@ -28710,7 +28908,10 @@
         <f>VLOOKUP(I58,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K58" s="117"/>
+      <c r="K58" s="126" t="str">
+        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L58" s="117"/>
       <c r="M58" s="117"/>
       <c r="N58" s="117"/>
@@ -28800,7 +29001,10 @@
         <f>VLOOKUP(I59,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
-      <c r="K59" s="117"/>
+      <c r="K59" s="126" t="str">
+        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L59" s="117"/>
       <c r="M59" s="117"/>
       <c r="N59" s="117"/>
@@ -28890,7 +29094,10 @@
         <f>VLOOKUP(I60,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K60" s="117"/>
+      <c r="K60" s="126" t="str">
+        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L60" s="117"/>
       <c r="M60" s="117"/>
       <c r="N60" s="117"/>
@@ -28980,7 +29187,10 @@
         <f>VLOOKUP(I61,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K61" s="117"/>
+      <c r="K61" s="126" t="str">
+        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L61" s="117"/>
       <c r="M61" s="117"/>
       <c r="N61" s="117"/>
@@ -29070,7 +29280,10 @@
         <f>VLOOKUP(I62,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K62" s="117"/>
+      <c r="K62" s="126" t="str">
+        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L62" s="117"/>
       <c r="M62" s="117"/>
       <c r="N62" s="117"/>
@@ -29160,7 +29373,10 @@
         <f>VLOOKUP(I63,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v>Business Audit captures all events that occur for a participant across a screening pathway e.g. digital communications, appointment attendance. It does this in a manner that prevents data tampering and is used for  non repudiation, clinical safety and identification and investigation of incidents.</v>
       </c>
-      <c r="K63" s="117"/>
+      <c r="K63" s="126" t="str">
+        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L63" s="117"/>
       <c r="M63" s="117"/>
       <c r="N63" s="117"/>
@@ -29250,7 +29466,10 @@
         <f>VLOOKUP(I64,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K64" s="117"/>
+      <c r="K64" s="126" t="str">
+        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L64" s="117"/>
       <c r="M64" s="117"/>
       <c r="N64" s="117"/>
@@ -29340,7 +29559,10 @@
         <f>VLOOKUP(I65,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
-      <c r="K65" s="117"/>
+      <c r="K65" s="126" t="str">
+        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <v>Operational Staff</v>
+      </c>
       <c r="L65" s="117"/>
       <c r="M65" s="117"/>
       <c r="N65" s="117"/>
@@ -29756,128 +29978,171 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8096783-64B1-C547-94F3-04D3BE1EF5B1}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" customWidth="1"/>
+    <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="337" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="180" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="178" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="177" t="s">
         <v>105</v>
       </c>
       <c r="B3" s="178" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="177" t="s">
         <v>110</v>
       </c>
       <c r="B4" s="178" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="183" t="s">
         <v>122</v>
       </c>
       <c r="B5" s="101" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="177" t="s">
         <v>126</v>
       </c>
       <c r="B6" s="178" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="177" t="s">
         <v>131</v>
       </c>
       <c r="B7" s="178" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="177" t="s">
         <v>137</v>
       </c>
       <c r="B8" s="178" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="177" t="s">
         <v>141</v>
       </c>
       <c r="B9" s="178" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="179" t="s">
         <v>216</v>
       </c>
       <c r="B10" s="178" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="177" t="s">
         <v>157</v>
       </c>
       <c r="B11" s="178" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="52" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="177" t="s">
         <v>172</v>
       </c>
       <c r="B12" s="178" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="154" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="177" t="s">
         <v>175</v>
       </c>
       <c r="B13" s="178" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="182" t="s">
         <v>186</v>
       </c>
       <c r="B14" s="181" t="s">
         <v>187</v>
+      </c>
+      <c r="C14" t="s">
+        <v>453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to naming to include numerical references
</commit_message>
<xml_diff>
--- a/data/BusinessCapabilitiesv0.1.xlsx
+++ b/data/BusinessCapabilitiesv0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leegath/LAG/Fathomatics/code/nhse/capabilitygenerator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA1B443-1E9B-C944-8F26-E94A411EEB75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF8654-F7D9-E742-8A79-6F8A41ED8535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="26580" activeTab="3" xr2:uid="{FB9E69F6-520F-B448-8326-5E7FF50D6D4B}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="Product Vision Map 2" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Capability Map Flattened'!$A$1:$J$65</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Capability Map Flattened'!$A$1:$K$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Product Definitions'!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Yellow postit notes'!$A$1:$D$1</definedName>
   </definedNames>
@@ -404,7 +404,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="481">
   <si>
     <t>Value Stream Stage</t>
   </si>
@@ -1375,8 +1375,302 @@
     <t>Capability Description</t>
   </si>
   <si>
+    <t>NHS UK</t>
+  </si>
+  <si>
+    <t>Cohorting as a Service</t>
+  </si>
+  <si>
+    <t>Drive outcome – Based on diagnosis, determine next best action</t>
+  </si>
+  <si>
+    <t>Access to personal dashboard: Provide participants with a centralised view of their screening journey.</t>
+  </si>
+  <si>
+    <t>Apply allocation model: Support different pathways having a different resource allocation algorithm</t>
+  </si>
+  <si>
+    <t>Appointment Administration: Ability to amend or cancel appointments by an internal team, including local capacity changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment choice: Present a set of appointment options to the participant </t>
+  </si>
+  <si>
+    <t>Appointment configuration: Set appointment slot durations based on participant needs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Appointment list: Supporting operational management of clinics </t>
+  </si>
+  <si>
+    <t>Appointment opportunity: Enable opportunistic screening in accessible locations (e.g., pharmacies).</t>
+  </si>
+  <si>
+    <t>Appointment reminder: Send reminders before scheduled appointments.</t>
+  </si>
+  <si>
+    <t>Appointments missed: Follow up on missed appointments to reschedule as needed.</t>
+  </si>
+  <si>
+    <t>Campaign analyses: Generate reports on campaign effectiveness across multiple channels.</t>
+  </si>
+  <si>
+    <t>Cohort creation: Identify eligible participants based on defined criteria.</t>
+  </si>
+  <si>
+    <t>Cohort exceptions: Manage participant inclusions/exclusions based on specific personal or situational factors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Communicate to GP - Send communication to the GP about the outcome </t>
+  </si>
+  <si>
+    <t>Communicate to participant - Apply the appropriate communication method for relaying the outcome</t>
+  </si>
+  <si>
+    <t>Conduct clinical investigation: Carry out and document the screening procedure (e.g., mammogram).</t>
+  </si>
+  <si>
+    <t>Correlation mining: Correlate non-engagement behavior with participant properties to inform pathway improvements.</t>
+  </si>
+  <si>
+    <t>Creating reassurance and support content: Develop educational materials to improve awareness and participation.</t>
+  </si>
+  <si>
+    <t>Data completeness checks: Validate accuracy of participant data and completeness of screening records.</t>
+  </si>
+  <si>
+    <t>Dataset publication: Make data available for researchers with appropriate anonymisation.</t>
+  </si>
+  <si>
+    <t>Declaring an incident: Initiate incident assessment and determine response level.</t>
+  </si>
+  <si>
+    <t>Determine available capacity: Devise a high level screening capacity plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External referral integration - Transimission of necessary information to support onward referral. Including any necessary communication </t>
+  </si>
+  <si>
+    <t>Forecast capacity requirements: Project resource needs based on expected demand.</t>
+  </si>
+  <si>
+    <t>Identify demand smoothing opportunities: Assess demand fluctuations to optimise resource use.</t>
+  </si>
+  <si>
+    <t>Identity and contact details checks: Verify participant identity and contact information.</t>
+  </si>
+  <si>
+    <t>Inbound Communications: Provide service for participants to request additional information and support</t>
+  </si>
+  <si>
+    <t>Individual risk assessment allocation: Use historical data to derive the optimal slot allocation for an individual</t>
+  </si>
+  <si>
+    <t>Investigations and remedial actions (safety incident): Conduct investigations and take corrective actions.</t>
+  </si>
+  <si>
+    <t>Kit fulfilment: Dispatch sample kits as required for participants.</t>
+  </si>
+  <si>
+    <t>Manage electronic interpretation (AI): Leverage AI for sample interpretation where applicable.</t>
+  </si>
+  <si>
+    <t>Manage sample interpretation (Lab - Human): Interpretation of samples by laboratory personnel.</t>
+  </si>
+  <si>
+    <t>Marketing campaigns: Plan, execute, and track campaigns to increase screening awareness.</t>
+  </si>
+  <si>
+    <t>Messaging matrix: Create marketing and promotional messaging tailored to different participant groups.</t>
+  </si>
+  <si>
+    <t>Multi variant testing:  Create new pathway trials to improve health outcomes</t>
+  </si>
+  <si>
+    <t>Non digital assistance: Provide ability to support non digital channels</t>
+  </si>
+  <si>
+    <t>Non repudiation: Capacity to track everything that has happened to an indivdual during a screening episode</t>
+  </si>
+  <si>
+    <t>Non-actioned reminder: Send a reminder for non-actioned appointments</t>
+  </si>
+  <si>
+    <t>Obtain informed consent: Collect participant consent for screening actions.</t>
+  </si>
+  <si>
+    <t>Operational KPI presentation: Present KPIs hierarchically for in-depth analysis.</t>
+  </si>
+  <si>
+    <t>Participant Appointment Administration:  Ability for a participant to review and change their upcoming appointments</t>
+  </si>
+  <si>
+    <t>Participant self referral: Ability to self refer into a programme</t>
+  </si>
+  <si>
+    <t>Pathway customisation: Easily modify pathways to improve efficacy and reach of screening programmes</t>
+  </si>
+  <si>
+    <t>Pathway view: Single dashboard view of participant flow within a screening pathway</t>
+  </si>
+  <si>
+    <t>Performance reporting: Generate service performance reports for NHS/public communication.</t>
+  </si>
+  <si>
+    <t>Pre-screen questionaire : Comeplete a pre-screening questionaire ahead of time</t>
+  </si>
+  <si>
+    <t>Pre-screen questionnaire recording: Ensure pre-screen information has been provided before the screening takes place</t>
+  </si>
+  <si>
+    <t>Preference management: Provide ability to manage preferences around reasonable adjustments</t>
+  </si>
+  <si>
+    <t>Provide access to supporting materials: Offer participants information to make informed choices.</t>
+  </si>
+  <si>
+    <t>Query facility: Enable ad hoc data queries based on user inputs.</t>
+  </si>
+  <si>
+    <t>Receive health need information: Gather information on health needs, including demographics and exclusions.</t>
+  </si>
+  <si>
+    <t>Receive supply-side information: Collect data on resources, assets, and capacity availability.</t>
+  </si>
+  <si>
+    <t>Record diagnosis: Based on findings, record a diagnosis against the participant's record</t>
+  </si>
+  <si>
+    <t>Review findings: Able to review all findings and history for a participant so as to make the right next decision</t>
+  </si>
+  <si>
+    <t>Sample receiving and tracking: Track samples and match them with participant data.</t>
+  </si>
+  <si>
+    <t>Select due participants: Select and update due participants</t>
+  </si>
+  <si>
+    <t>Self referral: Accept and validate a self referral request</t>
+  </si>
+  <si>
+    <t>Send appointment invitation: Notify participants of appointments via preferred channels.</t>
+  </si>
+  <si>
+    <t>Set modelling parameters: Define parameters for planning, including geographic and temporal scales.</t>
+  </si>
+  <si>
+    <t>Slot prioritisation factors: Adjust modelling based on reasonable adjustments characteristics</t>
+  </si>
+  <si>
+    <t>Technical checks: Verify participant eligibility and scheduling to ensure correct cohort inclusion.</t>
+  </si>
+  <si>
+    <t>Timed appointments allocation: Allocate specific time slots for participants.</t>
+  </si>
+  <si>
+    <t>Transaction history mining: Analyse participant interactions with the screening process to improve pathway efficiency.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update GP record - Update GP record with outcome </t>
+  </si>
+  <si>
+    <t>Product Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </t>
+  </si>
+  <si>
+    <t>#N/A</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>System User</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Participant, Staff users</t>
+  </si>
+  <si>
+    <t>Staff users, Secondary users</t>
+  </si>
+  <si>
+    <t>Participant users, Staff users, Secondary users</t>
+  </si>
+  <si>
+    <t>Secondary users</t>
+  </si>
+  <si>
+    <t>Participant users, Staff users, Tertiary users</t>
+  </si>
+  <si>
+    <t>Participant, Staff users, Tertiary users</t>
+  </si>
+  <si>
+    <t>S1. Plan pathway</t>
+  </si>
+  <si>
+    <t>S2. Invite and book participants</t>
+  </si>
+  <si>
+    <t>S3. Screen participant</t>
+  </si>
+  <si>
+    <t>S4. Manage outcome</t>
+  </si>
+  <si>
+    <t>S5. Monitor Pathway</t>
+  </si>
+  <si>
+    <t>C1 Design/optimise pathway</t>
+  </si>
+  <si>
+    <t>C2 Execute campaigns</t>
+  </si>
+  <si>
+    <t>C3 Forecast capacity and demand</t>
+  </si>
+  <si>
+    <t>C4 Define due participants</t>
+  </si>
+  <si>
+    <t>C5. Invite and book participants</t>
+  </si>
+  <si>
+    <t>C6 Engage participants</t>
+  </si>
+  <si>
+    <t>C7 Prepare participant</t>
+  </si>
+  <si>
+    <t>C8 Adminster clinical investigation</t>
+  </si>
+  <si>
+    <t>C9 Determine finding(s)</t>
+  </si>
+  <si>
+    <t>C10 Determine diagnosis</t>
+  </si>
+  <si>
+    <t>C11 Determine outcome</t>
+  </si>
+  <si>
+    <t>C12 Communicate outcome</t>
+  </si>
+  <si>
+    <t>C13 Track Performance</t>
+  </si>
+  <si>
+    <t>C14 Support Research</t>
+  </si>
+  <si>
+    <t>C15 Investigate Incidents</t>
+  </si>
+  <si>
     <r>
-      <t>Transaction history mining</t>
+      <t>C1.1 Transaction history mining</t>
     </r>
     <r>
       <rPr>
@@ -1390,7 +1684,7 @@
   </si>
   <si>
     <r>
-      <t>Correlation mining</t>
+      <t>C1.2 Correlation mining</t>
     </r>
     <r>
       <rPr>
@@ -1404,7 +1698,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Multi variant testing: </t>
+      <t xml:space="preserve">C1.3 Multi variant testing: </t>
     </r>
     <r>
       <rPr>
@@ -1418,7 +1712,7 @@
   </si>
   <si>
     <r>
-      <t>Pathway customisation</t>
+      <t>C1.4 Pathway customisation</t>
     </r>
     <r>
       <rPr>
@@ -1432,7 +1726,7 @@
   </si>
   <si>
     <r>
-      <t>Creating reassurance and support content</t>
+      <t>C2.1 Creating reassurance and support content</t>
     </r>
     <r>
       <rPr>
@@ -1445,11 +1739,8 @@
     </r>
   </si>
   <si>
-    <t>NHS UK</t>
-  </si>
-  <si>
     <r>
-      <t>Messaging matrix</t>
+      <t>C2.2 Messaging matrix</t>
     </r>
     <r>
       <rPr>
@@ -1463,7 +1754,7 @@
   </si>
   <si>
     <r>
-      <t>Marketing campaigns</t>
+      <t>C2.3 Marketing campaigns</t>
     </r>
     <r>
       <rPr>
@@ -1477,7 +1768,21 @@
   </si>
   <si>
     <r>
-      <t>Receive supply-side information</t>
+      <t>C2.4 Campaign analysis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Generate reports on campaign effectiveness across multiple channels.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C3.1 Receive supply-side information</t>
     </r>
     <r>
       <rPr>
@@ -1491,7 +1796,7 @@
   </si>
   <si>
     <r>
-      <t>Receive health need information</t>
+      <t>C3.2 Receive health need information</t>
     </r>
     <r>
       <rPr>
@@ -1505,7 +1810,7 @@
   </si>
   <si>
     <r>
-      <t>Set modelling parameters</t>
+      <t>C3.3 Set modelling parameters</t>
     </r>
     <r>
       <rPr>
@@ -1519,7 +1824,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Determine available capacity: </t>
+      <t xml:space="preserve">C3.4 Determine available capacity: </t>
     </r>
     <r>
       <rPr>
@@ -1532,7 +1837,7 @@
   </si>
   <si>
     <r>
-      <t>Forecast capacity requirements</t>
+      <t>C3.5 Forecast capacity requirements</t>
     </r>
     <r>
       <rPr>
@@ -1546,7 +1851,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Slot prioritisation factors: </t>
+      <t xml:space="preserve">C3.6 Slot prioritisation factors: </t>
     </r>
     <r>
       <rPr>
@@ -1559,7 +1864,7 @@
   </si>
   <si>
     <r>
-      <t>Identify demand smoothing opportunities</t>
+      <t>C3.7 Identify demand smoothing opportunities</t>
     </r>
     <r>
       <rPr>
@@ -1573,7 +1878,7 @@
   </si>
   <si>
     <r>
-      <t>Cohort creation</t>
+      <t>C4.1 Cohort creation</t>
     </r>
     <r>
       <rPr>
@@ -1586,11 +1891,8 @@
     </r>
   </si>
   <si>
-    <t>Cohorting as a Service</t>
-  </si>
-  <si>
     <r>
-      <t>Select due participants</t>
+      <t>C4.2 Select due participants</t>
     </r>
     <r>
       <rPr>
@@ -1604,7 +1906,7 @@
   </si>
   <si>
     <r>
-      <t>Self referral</t>
+      <t>C4.3 Self referral</t>
     </r>
     <r>
       <rPr>
@@ -1617,7 +1919,7 @@
   </si>
   <si>
     <r>
-      <t>Technical checks</t>
+      <t>C4.4 Technical checks</t>
     </r>
     <r>
       <rPr>
@@ -1631,7 +1933,7 @@
   </si>
   <si>
     <r>
-      <t>Data completeness checks</t>
+      <t>C4.5 Data completeness checks</t>
     </r>
     <r>
       <rPr>
@@ -1645,7 +1947,7 @@
   </si>
   <si>
     <r>
-      <t>Cohort exceptions</t>
+      <t>C4.6 Cohort exceptions</t>
     </r>
     <r>
       <rPr>
@@ -1659,7 +1961,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Apply allocation model: </t>
+      <t xml:space="preserve">C5.1 Apply allocation model: </t>
     </r>
     <r>
       <rPr>
@@ -1672,13 +1974,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Individual risk assessment allocation</t>
+      <t>C5.2 Individual risk assessment allocation</t>
     </r>
     <r>
       <rPr>
@@ -1691,7 +1987,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment configuration</t>
+      <t>C5.3 Appointment configuration</t>
     </r>
     <r>
       <rPr>
@@ -1705,7 +2001,7 @@
   </si>
   <si>
     <r>
-      <t>Timed appointments allocation</t>
+      <t>C5.4 Timed appointments allocation</t>
     </r>
     <r>
       <rPr>
@@ -1719,7 +2015,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment choice</t>
+      <t>C5.5 Appointment choice</t>
     </r>
     <r>
       <rPr>
@@ -1732,7 +2028,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment opportunity</t>
+      <t>C5.6 Appointment opportunity</t>
     </r>
     <r>
       <rPr>
@@ -1746,7 +2042,7 @@
   </si>
   <si>
     <r>
-      <t>Send appointment invitation</t>
+      <t>C5.7 Send appointment invitation</t>
     </r>
     <r>
       <rPr>
@@ -1760,13 +2056,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Access to personal dashboard</t>
+      <t>C6.1 Access to personal dashboard</t>
     </r>
     <r>
       <rPr>
@@ -1779,13 +2069,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Preference management:</t>
+      <t>C6.2 Preference management:</t>
     </r>
     <r>
       <rPr>
@@ -1798,13 +2082,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Participant self referral: </t>
+      <t xml:space="preserve">C6.3 Participant self referral: </t>
     </r>
     <r>
       <rPr>
@@ -1817,13 +2095,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Pre-screen questionaire</t>
+      <t>C6.4 Pre-screen questionaire</t>
     </r>
     <r>
       <rPr>
@@ -1836,7 +2108,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Participant Appointment Administration: </t>
+      <t xml:space="preserve">C6.5 Participant Appointment Administration: </t>
     </r>
     <r>
       <rPr>
@@ -1849,7 +2121,7 @@
   </si>
   <si>
     <r>
-      <t>Non-actioned reminder</t>
+      <t>C6.6 Non-actioned reminder</t>
     </r>
     <r>
       <rPr>
@@ -1862,7 +2134,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment reminder</t>
+      <t>C6.7 Appointment reminder</t>
     </r>
     <r>
       <rPr>
@@ -1876,7 +2148,7 @@
   </si>
   <si>
     <r>
-      <t>Appointments missed</t>
+      <t>C6.8 Appointments missed</t>
     </r>
     <r>
       <rPr>
@@ -1890,7 +2162,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment Administration:</t>
+      <t>C6.9 Appointment Administration:</t>
     </r>
     <r>
       <rPr>
@@ -1903,7 +2175,7 @@
   </si>
   <si>
     <r>
-      <t>Non digital assistance:</t>
+      <t>C6.10 Non digital assistance:</t>
     </r>
     <r>
       <rPr>
@@ -1916,7 +2188,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Inbound Communications: </t>
+      <t xml:space="preserve">C6.11 Inbound Communications: </t>
     </r>
     <r>
       <rPr>
@@ -1929,7 +2201,7 @@
   </si>
   <si>
     <r>
-      <t>Appointment list</t>
+      <t>C6.12 Appointment list</t>
     </r>
     <r>
       <rPr>
@@ -1942,7 +2214,7 @@
   </si>
   <si>
     <r>
-      <t>Identity and contact details checks</t>
+      <t>C7.1 Identity and contact details checks</t>
     </r>
     <r>
       <rPr>
@@ -1956,13 +2228,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Pre-screen questionnaire recording: </t>
+      <t xml:space="preserve">C7.2 Pre-screen questionnaire recording: </t>
     </r>
     <r>
       <rPr>
@@ -1975,7 +2241,7 @@
   </si>
   <si>
     <r>
-      <t>Obtain informed consent</t>
+      <t>C7.3 Obtain informed consent</t>
     </r>
     <r>
       <rPr>
@@ -1989,7 +2255,7 @@
   </si>
   <si>
     <r>
-      <t>Provide access to supporting materials</t>
+      <t>C7.4 Provide access to supporting materials</t>
     </r>
     <r>
       <rPr>
@@ -2003,13 +2269,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Conduct clinical investigation</t>
+      <t>C8.1 Conduct clinical investigation</t>
     </r>
     <r>
       <rPr>
@@ -2022,7 +2282,7 @@
   </si>
   <si>
     <r>
-      <t>Sample receiving and tracking</t>
+      <t>C8.2 Sample receiving and tracking</t>
     </r>
     <r>
       <rPr>
@@ -2036,7 +2296,7 @@
   </si>
   <si>
     <r>
-      <t>Kit fulfilment</t>
+      <t>C8.3 Kit fulfilment</t>
     </r>
     <r>
       <rPr>
@@ -2050,13 +2310,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Manage sample interpretation (Lab - Human)</t>
+      <t>C9.1 Manage sample interpretation (Lab - Human)</t>
     </r>
     <r>
       <rPr>
@@ -2069,13 +2323,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Manage electronic interpretation (AI)</t>
+      <t>C9.2 Manage electronic interpretation (AI)</t>
     </r>
     <r>
       <rPr>
@@ -2088,13 +2336,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Review findings: </t>
+      <t xml:space="preserve">C10.1 Review findings: </t>
     </r>
     <r>
       <rPr>
@@ -2107,13 +2349,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Record diagnosis:</t>
+      <t>C10.2 Record diagnosis:</t>
     </r>
     <r>
       <rPr>
@@ -2125,11 +2361,80 @@
     </r>
   </si>
   <si>
-    <t>Drive outcome – Based on diagnosis, determine next best action</t>
-  </si>
-  <si>
     <r>
-      <t>Operational KPI presentation</t>
+      <t>C11.1 External referral integration:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Transimission of necessary information to support onward referral. Including any necessary communication </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>C11.2 Drive outcome:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve"> Based on diagnosis, determine next best action</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C12.1 Update GP record: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Update GP record with outcome </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C12.2 Communicate to GP: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t xml:space="preserve">Send communication to the GP about the outcome </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">C12.3 Communicate to participant: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+      </rPr>
+      <t>Apply the appropriate communication method for relaying the outcome</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C13.1 Operational KPI presentation</t>
     </r>
     <r>
       <rPr>
@@ -2143,7 +2448,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Pathway view: </t>
+      <t xml:space="preserve">C13.2 Pathway view: </t>
     </r>
     <r>
       <rPr>
@@ -2156,7 +2461,7 @@
   </si>
   <si>
     <r>
-      <t>Performance reporting</t>
+      <t>C13.3 Performance reporting</t>
     </r>
     <r>
       <rPr>
@@ -2170,7 +2475,7 @@
   </si>
   <si>
     <r>
-      <t>Dataset publication</t>
+      <t>C14.1 Dataset publication</t>
     </r>
     <r>
       <rPr>
@@ -2184,7 +2489,7 @@
   </si>
   <si>
     <r>
-      <t>Query facility</t>
+      <t>C14.2 Query facility</t>
     </r>
     <r>
       <rPr>
@@ -2198,13 +2503,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Non repudiation:</t>
+      <t>C15.1 Non repudiation:</t>
     </r>
     <r>
       <rPr>
@@ -2217,7 +2516,7 @@
   </si>
   <si>
     <r>
-      <t>Declaring an incident</t>
+      <t>C15.2 Declaring an incident</t>
     </r>
     <r>
       <rPr>
@@ -2231,7 +2530,7 @@
   </si>
   <si>
     <r>
-      <t>Investigations and remedial actions (safety incident)</t>
+      <t>C15.3 Investigations and remedial actions (safety incident)</t>
     </r>
     <r>
       <rPr>
@@ -2242,295 +2541,6 @@
       </rPr>
       <t>: Conduct investigations and take corrective actions.</t>
     </r>
-  </si>
-  <si>
-    <t>Access to personal dashboard: Provide participants with a centralised view of their screening journey.</t>
-  </si>
-  <si>
-    <t>Apply allocation model: Support different pathways having a different resource allocation algorithm</t>
-  </si>
-  <si>
-    <t>Appointment Administration: Ability to amend or cancel appointments by an internal team, including local capacity changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appointment choice: Present a set of appointment options to the participant </t>
-  </si>
-  <si>
-    <t>Appointment configuration: Set appointment slot durations based on participant needs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Appointment list: Supporting operational management of clinics </t>
-  </si>
-  <si>
-    <t>Appointment opportunity: Enable opportunistic screening in accessible locations (e.g., pharmacies).</t>
-  </si>
-  <si>
-    <t>Appointment reminder: Send reminders before scheduled appointments.</t>
-  </si>
-  <si>
-    <t>Appointments missed: Follow up on missed appointments to reschedule as needed.</t>
-  </si>
-  <si>
-    <t>Campaign analyses: Generate reports on campaign effectiveness across multiple channels.</t>
-  </si>
-  <si>
-    <t>Cohort creation: Identify eligible participants based on defined criteria.</t>
-  </si>
-  <si>
-    <t>Cohort exceptions: Manage participant inclusions/exclusions based on specific personal or situational factors.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Communicate to GP - Send communication to the GP about the outcome </t>
-  </si>
-  <si>
-    <t>Communicate to participant - Apply the appropriate communication method for relaying the outcome</t>
-  </si>
-  <si>
-    <t>Conduct clinical investigation: Carry out and document the screening procedure (e.g., mammogram).</t>
-  </si>
-  <si>
-    <t>Correlation mining: Correlate non-engagement behavior with participant properties to inform pathway improvements.</t>
-  </si>
-  <si>
-    <t>Creating reassurance and support content: Develop educational materials to improve awareness and participation.</t>
-  </si>
-  <si>
-    <t>Data completeness checks: Validate accuracy of participant data and completeness of screening records.</t>
-  </si>
-  <si>
-    <t>Dataset publication: Make data available for researchers with appropriate anonymisation.</t>
-  </si>
-  <si>
-    <t>Declaring an incident: Initiate incident assessment and determine response level.</t>
-  </si>
-  <si>
-    <t>Determine available capacity: Devise a high level screening capacity plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">External referral integration - Transimission of necessary information to support onward referral. Including any necessary communication </t>
-  </si>
-  <si>
-    <t>Forecast capacity requirements: Project resource needs based on expected demand.</t>
-  </si>
-  <si>
-    <t>Identify demand smoothing opportunities: Assess demand fluctuations to optimise resource use.</t>
-  </si>
-  <si>
-    <t>Identity and contact details checks: Verify participant identity and contact information.</t>
-  </si>
-  <si>
-    <t>Inbound Communications: Provide service for participants to request additional information and support</t>
-  </si>
-  <si>
-    <t>Individual risk assessment allocation: Use historical data to derive the optimal slot allocation for an individual</t>
-  </si>
-  <si>
-    <t>Investigations and remedial actions (safety incident): Conduct investigations and take corrective actions.</t>
-  </si>
-  <si>
-    <t>Kit fulfilment: Dispatch sample kits as required for participants.</t>
-  </si>
-  <si>
-    <t>Manage electronic interpretation (AI): Leverage AI for sample interpretation where applicable.</t>
-  </si>
-  <si>
-    <t>Manage sample interpretation (Lab - Human): Interpretation of samples by laboratory personnel.</t>
-  </si>
-  <si>
-    <t>Marketing campaigns: Plan, execute, and track campaigns to increase screening awareness.</t>
-  </si>
-  <si>
-    <t>Messaging matrix: Create marketing and promotional messaging tailored to different participant groups.</t>
-  </si>
-  <si>
-    <t>Multi variant testing:  Create new pathway trials to improve health outcomes</t>
-  </si>
-  <si>
-    <t>Non digital assistance: Provide ability to support non digital channels</t>
-  </si>
-  <si>
-    <t>Non repudiation: Capacity to track everything that has happened to an indivdual during a screening episode</t>
-  </si>
-  <si>
-    <t>Non-actioned reminder: Send a reminder for non-actioned appointments</t>
-  </si>
-  <si>
-    <t>Obtain informed consent: Collect participant consent for screening actions.</t>
-  </si>
-  <si>
-    <t>Operational KPI presentation: Present KPIs hierarchically for in-depth analysis.</t>
-  </si>
-  <si>
-    <t>Participant Appointment Administration:  Ability for a participant to review and change their upcoming appointments</t>
-  </si>
-  <si>
-    <t>Participant self referral: Ability to self refer into a programme</t>
-  </si>
-  <si>
-    <t>Pathway customisation: Easily modify pathways to improve efficacy and reach of screening programmes</t>
-  </si>
-  <si>
-    <t>Pathway view: Single dashboard view of participant flow within a screening pathway</t>
-  </si>
-  <si>
-    <t>Performance reporting: Generate service performance reports for NHS/public communication.</t>
-  </si>
-  <si>
-    <t>Pre-screen questionaire : Comeplete a pre-screening questionaire ahead of time</t>
-  </si>
-  <si>
-    <t>Pre-screen questionnaire recording: Ensure pre-screen information has been provided before the screening takes place</t>
-  </si>
-  <si>
-    <t>Preference management: Provide ability to manage preferences around reasonable adjustments</t>
-  </si>
-  <si>
-    <t>Provide access to supporting materials: Offer participants information to make informed choices.</t>
-  </si>
-  <si>
-    <t>Query facility: Enable ad hoc data queries based on user inputs.</t>
-  </si>
-  <si>
-    <t>Receive health need information: Gather information on health needs, including demographics and exclusions.</t>
-  </si>
-  <si>
-    <t>Receive supply-side information: Collect data on resources, assets, and capacity availability.</t>
-  </si>
-  <si>
-    <t>Record diagnosis: Based on findings, record a diagnosis against the participant's record</t>
-  </si>
-  <si>
-    <t>Review findings: Able to review all findings and history for a participant so as to make the right next decision</t>
-  </si>
-  <si>
-    <t>Sample receiving and tracking: Track samples and match them with participant data.</t>
-  </si>
-  <si>
-    <t>Select due participants: Select and update due participants</t>
-  </si>
-  <si>
-    <t>Self referral: Accept and validate a self referral request</t>
-  </si>
-  <si>
-    <t>Send appointment invitation: Notify participants of appointments via preferred channels.</t>
-  </si>
-  <si>
-    <t>Set modelling parameters: Define parameters for planning, including geographic and temporal scales.</t>
-  </si>
-  <si>
-    <t>Slot prioritisation factors: Adjust modelling based on reasonable adjustments characteristics</t>
-  </si>
-  <si>
-    <t>Technical checks: Verify participant eligibility and scheduling to ensure correct cohort inclusion.</t>
-  </si>
-  <si>
-    <t>Timed appointments allocation: Allocate specific time slots for participants.</t>
-  </si>
-  <si>
-    <t>Transaction history mining: Analyse participant interactions with the screening process to improve pathway efficiency.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Update GP record - Update GP record with outcome </t>
-  </si>
-  <si>
-    <t>Product Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </t>
-  </si>
-  <si>
-    <t>#N/A</t>
-  </si>
-  <si>
-    <r>
-      <t>Campaign analysis</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>: Generate reports on campaign effectiveness across multiple channels.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>External referral integration:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> Transimission of necessary information to support onward referral. Including any necessary communication </t>
-    </r>
-  </si>
-  <si>
-    <t>Drive outcome: Based on diagnosis, determine next best action</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Update GP record: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Update GP record with outcome </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Communicate to GP: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t xml:space="preserve">Send communication to the GP about the outcome </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Communicate to participant: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Narrow"/>
-      </rPr>
-      <t>Apply the appropriate communication method for relaying the outcome</t>
-    </r>
-  </si>
-  <si>
-    <t>5.2 Support Research</t>
-  </si>
-  <si>
-    <t>Participant, Clinical Staff, Operational Staff</t>
-  </si>
-  <si>
-    <t>Users</t>
-  </si>
-  <si>
-    <t>Operational Staff</t>
-  </si>
-  <si>
-    <t>System User</t>
-  </si>
-  <si>
-    <t>Participant, Operational Staff</t>
-  </si>
-  <si>
-    <t>User</t>
   </si>
 </sst>
 </file>
@@ -23558,9 +23568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771BD26-5CB2-F242-A0FA-A4D8589272A0}">
   <dimension ref="A1:BO73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K66" sqref="K66"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23606,10 +23616,10 @@
         <v>82</v>
       </c>
       <c r="J1" s="114" t="s">
-        <v>443</v>
+        <v>385</v>
       </c>
       <c r="K1" s="338" t="s">
-        <v>458</v>
+        <v>390</v>
       </c>
       <c r="L1" s="114"/>
       <c r="M1" s="114"/>
@@ -23668,9 +23678,9 @@
       <c r="BN1" s="114"/>
       <c r="BO1" s="114"/>
     </row>
-    <row r="2" spans="1:67" s="1" customFormat="1" ht="204" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:67" s="1" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" s="108" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B2" s="113" t="s">
         <v>8</v>
@@ -23679,7 +23689,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="112" t="s">
-        <v>10</v>
+        <v>402</v>
       </c>
       <c r="E2" s="143" t="s">
         <v>12</v>
@@ -23691,7 +23701,7 @@
         <v>13</v>
       </c>
       <c r="H2" s="109" t="s">
-        <v>319</v>
+        <v>417</v>
       </c>
       <c r="I2" s="129" t="s">
         <v>87</v>
@@ -23702,7 +23712,7 @@
       </c>
       <c r="K2" s="126" t="str">
         <f>VLOOKUP(I2,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L2" s="114"/>
       <c r="M2" s="114"/>
@@ -23763,7 +23773,7 @@
     </row>
     <row r="3" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B3" s="116" t="s">
         <v>8</v>
@@ -23772,7 +23782,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="115" t="s">
-        <v>10</v>
+        <v>402</v>
       </c>
       <c r="E3" s="144" t="s">
         <v>12</v>
@@ -23784,7 +23794,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="110" t="s">
-        <v>320</v>
+        <v>418</v>
       </c>
       <c r="I3" s="129" t="s">
         <v>87</v>
@@ -23795,7 +23805,7 @@
       </c>
       <c r="K3" s="126" t="str">
         <f>VLOOKUP(I3,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L3" s="114"/>
       <c r="M3" s="114"/>
@@ -23856,7 +23866,7 @@
     </row>
     <row r="4" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A4" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B4" s="116" t="s">
         <v>8</v>
@@ -23865,7 +23875,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="115" t="s">
-        <v>10</v>
+        <v>402</v>
       </c>
       <c r="E4" s="144" t="s">
         <v>12</v>
@@ -23877,7 +23887,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="110" t="s">
-        <v>321</v>
+        <v>419</v>
       </c>
       <c r="I4" s="131" t="s">
         <v>175</v>
@@ -23888,7 +23898,7 @@
       </c>
       <c r="K4" s="126" t="str">
         <f>VLOOKUP(I4,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L4" s="114"/>
       <c r="M4" s="114"/>
@@ -23949,7 +23959,7 @@
     </row>
     <row r="5" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A5" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B5" s="116" t="s">
         <v>8</v>
@@ -23958,7 +23968,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="115" t="s">
-        <v>10</v>
+        <v>402</v>
       </c>
       <c r="E5" s="144" t="s">
         <v>12</v>
@@ -23970,7 +23980,7 @@
         <v>13</v>
       </c>
       <c r="H5" s="110" t="s">
-        <v>322</v>
+        <v>420</v>
       </c>
       <c r="I5" s="131" t="s">
         <v>175</v>
@@ -23981,7 +23991,7 @@
       </c>
       <c r="K5" s="126" t="str">
         <f>VLOOKUP(I5,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L5" s="117"/>
       <c r="M5" s="117"/>
@@ -24042,7 +24052,7 @@
     </row>
     <row r="6" spans="1:67" s="7" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B6" s="116" t="s">
         <v>8</v>
@@ -24051,7 +24061,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="115" t="s">
-        <v>14</v>
+        <v>403</v>
       </c>
       <c r="E6" s="144" t="s">
         <v>15</v>
@@ -24063,10 +24073,10 @@
         <v>17</v>
       </c>
       <c r="H6" s="110" t="s">
-        <v>323</v>
+        <v>421</v>
       </c>
       <c r="I6" s="131" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J6" s="126" t="e">
         <f>VLOOKUP(I6,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
@@ -24135,7 +24145,7 @@
     </row>
     <row r="7" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A7" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B7" s="116" t="s">
         <v>8</v>
@@ -24144,7 +24154,7 @@
         <v>9</v>
       </c>
       <c r="D7" s="115" t="s">
-        <v>14</v>
+        <v>403</v>
       </c>
       <c r="E7" s="144" t="s">
         <v>15</v>
@@ -24156,7 +24166,7 @@
         <v>17</v>
       </c>
       <c r="H7" s="110" t="s">
-        <v>325</v>
+        <v>422</v>
       </c>
       <c r="I7" s="131" t="s">
         <v>126</v>
@@ -24167,7 +24177,7 @@
       </c>
       <c r="K7" s="126" t="str">
         <f>VLOOKUP(I7,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L7" s="117"/>
       <c r="M7" s="117"/>
@@ -24228,7 +24238,7 @@
     </row>
     <row r="8" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A8" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B8" s="116" t="s">
         <v>8</v>
@@ -24237,7 +24247,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="115" t="s">
-        <v>14</v>
+        <v>403</v>
       </c>
       <c r="E8" s="144" t="s">
         <v>15</v>
@@ -24249,7 +24259,7 @@
         <v>17</v>
       </c>
       <c r="H8" s="110" t="s">
-        <v>326</v>
+        <v>423</v>
       </c>
       <c r="I8" s="131" t="s">
         <v>126</v>
@@ -24260,7 +24270,7 @@
       </c>
       <c r="K8" s="126" t="str">
         <f>VLOOKUP(I8,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L8" s="117"/>
       <c r="M8" s="117"/>
@@ -24321,7 +24331,7 @@
     </row>
     <row r="9" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B9" s="116" t="s">
         <v>8</v>
@@ -24330,7 +24340,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="115" t="s">
-        <v>14</v>
+        <v>403</v>
       </c>
       <c r="E9" s="144" t="s">
         <v>15</v>
@@ -24342,7 +24352,7 @@
         <v>17</v>
       </c>
       <c r="H9" s="110" t="s">
-        <v>446</v>
+        <v>424</v>
       </c>
       <c r="I9" s="131" t="s">
         <v>87</v>
@@ -24353,7 +24363,7 @@
       </c>
       <c r="K9" s="126" t="str">
         <f>VLOOKUP(I9,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L9" s="117"/>
       <c r="M9" s="117"/>
@@ -24414,7 +24424,7 @@
     </row>
     <row r="10" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A10" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B10" s="116" t="s">
         <v>8</v>
@@ -24423,7 +24433,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E10" s="144" t="s">
         <v>19</v>
@@ -24435,7 +24445,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="110" t="s">
-        <v>327</v>
+        <v>425</v>
       </c>
       <c r="I10" s="131" t="s">
         <v>137</v>
@@ -24446,7 +24456,7 @@
       </c>
       <c r="K10" s="126" t="str">
         <f>VLOOKUP(I10,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L10" s="117"/>
       <c r="M10" s="117"/>
@@ -24507,7 +24517,7 @@
     </row>
     <row r="11" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A11" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B11" s="116" t="s">
         <v>8</v>
@@ -24516,7 +24526,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E11" s="144" t="s">
         <v>19</v>
@@ -24528,7 +24538,7 @@
         <v>21</v>
       </c>
       <c r="H11" s="110" t="s">
-        <v>328</v>
+        <v>426</v>
       </c>
       <c r="I11" s="131" t="s">
         <v>141</v>
@@ -24539,7 +24549,7 @@
       </c>
       <c r="K11" s="126" t="str">
         <f>VLOOKUP(I11,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L11" s="117"/>
       <c r="M11" s="117"/>
@@ -24600,7 +24610,7 @@
     </row>
     <row r="12" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A12" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B12" s="116" t="s">
         <v>8</v>
@@ -24609,7 +24619,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E12" s="144" t="s">
         <v>19</v>
@@ -24621,7 +24631,7 @@
         <v>21</v>
       </c>
       <c r="H12" s="110" t="s">
-        <v>329</v>
+        <v>427</v>
       </c>
       <c r="I12" s="131" t="s">
         <v>131</v>
@@ -24632,7 +24642,7 @@
       </c>
       <c r="K12" s="126" t="str">
         <f>VLOOKUP(I12,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L12" s="117"/>
       <c r="M12" s="117"/>
@@ -24693,7 +24703,7 @@
     </row>
     <row r="13" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A13" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B13" s="116" t="s">
         <v>8</v>
@@ -24702,7 +24712,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E13" s="144" t="s">
         <v>19</v>
@@ -24714,7 +24724,7 @@
         <v>21</v>
       </c>
       <c r="H13" s="111" t="s">
-        <v>330</v>
+        <v>428</v>
       </c>
       <c r="I13" s="131" t="s">
         <v>137</v>
@@ -24725,7 +24735,7 @@
       </c>
       <c r="K13" s="126" t="str">
         <f>VLOOKUP(I13,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L13" s="117"/>
       <c r="M13" s="117"/>
@@ -24786,7 +24796,7 @@
     </row>
     <row r="14" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A14" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B14" s="116" t="s">
         <v>8</v>
@@ -24795,7 +24805,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E14" s="144" t="s">
         <v>19</v>
@@ -24807,7 +24817,7 @@
         <v>21</v>
       </c>
       <c r="H14" s="110" t="s">
-        <v>331</v>
+        <v>429</v>
       </c>
       <c r="I14" s="131" t="s">
         <v>131</v>
@@ -24818,7 +24828,7 @@
       </c>
       <c r="K14" s="126" t="str">
         <f>VLOOKUP(I14,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L14" s="117"/>
       <c r="M14" s="117"/>
@@ -24879,7 +24889,7 @@
     </row>
     <row r="15" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A15" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B15" s="116" t="s">
         <v>8</v>
@@ -24888,7 +24898,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E15" s="144" t="s">
         <v>19</v>
@@ -24900,7 +24910,7 @@
         <v>21</v>
       </c>
       <c r="H15" s="111" t="s">
-        <v>332</v>
+        <v>430</v>
       </c>
       <c r="I15" s="131" t="s">
         <v>131</v>
@@ -24911,7 +24921,7 @@
       </c>
       <c r="K15" s="126" t="str">
         <f>VLOOKUP(I15,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L15" s="117"/>
       <c r="M15" s="117"/>
@@ -24972,7 +24982,7 @@
     </row>
     <row r="16" spans="1:67" s="7" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A16" s="130" t="s">
-        <v>7</v>
+        <v>397</v>
       </c>
       <c r="B16" s="116" t="s">
         <v>8</v>
@@ -24981,7 +24991,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="115" t="s">
-        <v>18</v>
+        <v>404</v>
       </c>
       <c r="E16" s="144" t="s">
         <v>19</v>
@@ -24993,7 +25003,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="110" t="s">
-        <v>333</v>
+        <v>431</v>
       </c>
       <c r="I16" s="131" t="s">
         <v>131</v>
@@ -25004,7 +25014,7 @@
       </c>
       <c r="K16" s="126" t="str">
         <f>VLOOKUP(I16,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L16" s="117"/>
       <c r="M16" s="117"/>
@@ -25065,7 +25075,7 @@
     </row>
     <row r="17" spans="1:67" s="7" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B17" s="119" t="s">
         <v>23</v>
@@ -25074,7 +25084,7 @@
         <v>24</v>
       </c>
       <c r="D17" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E17" s="145" t="s">
         <v>26</v>
@@ -25086,10 +25096,10 @@
         <v>28</v>
       </c>
       <c r="H17" s="167" t="s">
-        <v>334</v>
+        <v>432</v>
       </c>
       <c r="I17" s="133" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="J17" s="126" t="e">
         <f>VLOOKUP(I17,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
@@ -25158,7 +25168,7 @@
     </row>
     <row r="18" spans="1:67" s="7" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A18" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B18" s="119" t="s">
         <v>23</v>
@@ -25167,7 +25177,7 @@
         <v>24</v>
       </c>
       <c r="D18" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E18" s="145" t="s">
         <v>26</v>
@@ -25179,7 +25189,7 @@
         <v>28</v>
       </c>
       <c r="H18" s="167" t="s">
-        <v>336</v>
+        <v>433</v>
       </c>
       <c r="I18" s="133" t="s">
         <v>175</v>
@@ -25190,7 +25200,7 @@
       </c>
       <c r="K18" s="126" t="str">
         <f>VLOOKUP(I18,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L18" s="117"/>
       <c r="M18" s="117"/>
@@ -25251,7 +25261,7 @@
     </row>
     <row r="19" spans="1:67" s="12" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B19" s="119" t="s">
         <v>23</v>
@@ -25260,7 +25270,7 @@
         <v>24</v>
       </c>
       <c r="D19" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E19" s="145" t="s">
         <v>26</v>
@@ -25272,7 +25282,7 @@
         <v>28</v>
       </c>
       <c r="H19" s="168" t="s">
-        <v>337</v>
+        <v>434</v>
       </c>
       <c r="I19" s="133" t="s">
         <v>141</v>
@@ -25283,7 +25293,7 @@
       </c>
       <c r="K19" s="126" t="str">
         <f>VLOOKUP(I19,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L19" s="117"/>
       <c r="M19" s="117"/>
@@ -25344,7 +25354,7 @@
     </row>
     <row r="20" spans="1:67" s="12" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B20" s="119" t="s">
         <v>23</v>
@@ -25353,7 +25363,7 @@
         <v>24</v>
       </c>
       <c r="D20" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E20" s="145" t="s">
         <v>26</v>
@@ -25365,7 +25375,7 @@
         <v>28</v>
       </c>
       <c r="H20" s="167" t="s">
-        <v>338</v>
+        <v>435</v>
       </c>
       <c r="I20" s="133" t="s">
         <v>141</v>
@@ -25376,7 +25386,7 @@
       </c>
       <c r="K20" s="126" t="str">
         <f>VLOOKUP(I20,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L20" s="117"/>
       <c r="M20" s="117"/>
@@ -25437,7 +25447,7 @@
     </row>
     <row r="21" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A21" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B21" s="119" t="s">
         <v>23</v>
@@ -25446,7 +25456,7 @@
         <v>24</v>
       </c>
       <c r="D21" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E21" s="145" t="s">
         <v>26</v>
@@ -25458,7 +25468,7 @@
         <v>28</v>
       </c>
       <c r="H21" s="167" t="s">
-        <v>339</v>
+        <v>436</v>
       </c>
       <c r="I21" s="133" t="s">
         <v>141</v>
@@ -25469,7 +25479,7 @@
       </c>
       <c r="K21" s="126" t="str">
         <f>VLOOKUP(I21,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L21" s="117"/>
       <c r="M21" s="117"/>
@@ -25530,7 +25540,7 @@
     </row>
     <row r="22" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A22" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B22" s="119" t="s">
         <v>23</v>
@@ -25539,7 +25549,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="118" t="s">
-        <v>25</v>
+        <v>405</v>
       </c>
       <c r="E22" s="145" t="s">
         <v>26</v>
@@ -25551,7 +25561,7 @@
         <v>28</v>
       </c>
       <c r="H22" s="167" t="s">
-        <v>340</v>
+        <v>437</v>
       </c>
       <c r="I22" s="133" t="s">
         <v>141</v>
@@ -25562,7 +25572,7 @@
       </c>
       <c r="K22" s="126" t="str">
         <f>VLOOKUP(I22,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L22" s="117"/>
       <c r="M22" s="117"/>
@@ -25623,7 +25633,7 @@
     </row>
     <row r="23" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A23" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B23" s="119" t="s">
         <v>23</v>
@@ -25632,7 +25642,7 @@
         <v>24</v>
       </c>
       <c r="D23" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E23" s="145" t="s">
         <v>30</v>
@@ -25644,7 +25654,7 @@
         <v>32</v>
       </c>
       <c r="H23" s="168" t="s">
-        <v>341</v>
+        <v>438</v>
       </c>
       <c r="I23" s="133" t="s">
         <v>105</v>
@@ -25716,7 +25726,7 @@
     </row>
     <row r="24" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A24" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B24" s="119" t="s">
         <v>23</v>
@@ -25725,7 +25735,7 @@
         <v>24</v>
       </c>
       <c r="D24" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E24" s="145" t="s">
         <v>30</v>
@@ -25737,7 +25747,7 @@
         <v>32</v>
       </c>
       <c r="H24" s="168" t="s">
-        <v>342</v>
+        <v>439</v>
       </c>
       <c r="I24" s="133" t="s">
         <v>105</v>
@@ -25809,7 +25819,7 @@
     </row>
     <row r="25" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A25" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B25" s="119" t="s">
         <v>23</v>
@@ -25818,7 +25828,7 @@
         <v>24</v>
       </c>
       <c r="D25" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E25" s="145" t="s">
         <v>30</v>
@@ -25830,7 +25840,7 @@
         <v>32</v>
       </c>
       <c r="H25" s="167" t="s">
-        <v>343</v>
+        <v>440</v>
       </c>
       <c r="I25" s="133" t="s">
         <v>110</v>
@@ -25841,7 +25851,7 @@
       </c>
       <c r="K25" s="126" t="str">
         <f>VLOOKUP(I25,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L25" s="117"/>
       <c r="M25" s="117"/>
@@ -25902,7 +25912,7 @@
     </row>
     <row r="26" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A26" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B26" s="119" t="s">
         <v>23</v>
@@ -25911,7 +25921,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E26" s="145" t="s">
         <v>30</v>
@@ -25923,7 +25933,7 @@
         <v>32</v>
       </c>
       <c r="H26" s="167" t="s">
-        <v>344</v>
+        <v>441</v>
       </c>
       <c r="I26" s="133" t="s">
         <v>110</v>
@@ -25934,7 +25944,7 @@
       </c>
       <c r="K26" s="126" t="str">
         <f>VLOOKUP(I26,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L26" s="117"/>
       <c r="M26" s="117"/>
@@ -25995,7 +26005,7 @@
     </row>
     <row r="27" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A27" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B27" s="119" t="s">
         <v>23</v>
@@ -26004,7 +26014,7 @@
         <v>24</v>
       </c>
       <c r="D27" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E27" s="145" t="s">
         <v>30</v>
@@ -26016,7 +26026,7 @@
         <v>32</v>
       </c>
       <c r="H27" s="168" t="s">
-        <v>345</v>
+        <v>442</v>
       </c>
       <c r="I27" s="133" t="s">
         <v>110</v>
@@ -26027,7 +26037,7 @@
       </c>
       <c r="K27" s="126" t="str">
         <f>VLOOKUP(I27,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L27" s="117"/>
       <c r="M27" s="117"/>
@@ -26088,7 +26098,7 @@
     </row>
     <row r="28" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A28" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B28" s="119" t="s">
         <v>23</v>
@@ -26097,7 +26107,7 @@
         <v>24</v>
       </c>
       <c r="D28" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E28" s="145" t="s">
         <v>30</v>
@@ -26109,7 +26119,7 @@
         <v>32</v>
       </c>
       <c r="H28" s="167" t="s">
-        <v>346</v>
+        <v>443</v>
       </c>
       <c r="I28" s="133" t="s">
         <v>110</v>
@@ -26120,7 +26130,7 @@
       </c>
       <c r="K28" s="126" t="str">
         <f>VLOOKUP(I28,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L28" s="117"/>
       <c r="M28" s="117"/>
@@ -26181,7 +26191,7 @@
     </row>
     <row r="29" spans="1:67" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A29" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B29" s="119" t="s">
         <v>23</v>
@@ -26190,7 +26200,7 @@
         <v>24</v>
       </c>
       <c r="D29" s="118" t="s">
-        <v>29</v>
+        <v>406</v>
       </c>
       <c r="E29" s="145" t="s">
         <v>30</v>
@@ -26202,7 +26212,7 @@
         <v>32</v>
       </c>
       <c r="H29" s="167" t="s">
-        <v>347</v>
+        <v>444</v>
       </c>
       <c r="I29" s="133" t="s">
         <v>216</v>
@@ -26213,7 +26223,7 @@
       </c>
       <c r="K29" s="126" t="str">
         <f>VLOOKUP(I29,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L29" s="117"/>
       <c r="M29" s="117"/>
@@ -26274,7 +26284,7 @@
     </row>
     <row r="30" spans="1:67" s="12" customFormat="1" ht="103" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B30" s="119" t="s">
         <v>23</v>
@@ -26283,7 +26293,7 @@
         <v>24</v>
       </c>
       <c r="D30" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E30" s="145" t="s">
         <v>34</v>
@@ -26295,7 +26305,7 @@
         <v>36</v>
       </c>
       <c r="H30" s="168" t="s">
-        <v>348</v>
+        <v>445</v>
       </c>
       <c r="I30" s="133" t="s">
         <v>157</v>
@@ -26306,7 +26316,7 @@
       </c>
       <c r="K30" s="126" t="str">
         <f>VLOOKUP(I30,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L30" s="117"/>
       <c r="M30" s="117"/>
@@ -26367,7 +26377,7 @@
     </row>
     <row r="31" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A31" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B31" s="119" t="s">
         <v>23</v>
@@ -26376,7 +26386,7 @@
         <v>24</v>
       </c>
       <c r="D31" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E31" s="145" t="s">
         <v>34</v>
@@ -26388,7 +26398,7 @@
         <v>36</v>
       </c>
       <c r="H31" s="168" t="s">
-        <v>349</v>
+        <v>446</v>
       </c>
       <c r="I31" s="133" t="s">
         <v>157</v>
@@ -26399,7 +26409,7 @@
       </c>
       <c r="K31" s="126" t="str">
         <f>VLOOKUP(I31,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L31" s="117"/>
       <c r="M31" s="117"/>
@@ -26460,7 +26470,7 @@
     </row>
     <row r="32" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A32" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B32" s="119" t="s">
         <v>23</v>
@@ -26469,7 +26479,7 @@
         <v>24</v>
       </c>
       <c r="D32" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E32" s="145" t="s">
         <v>34</v>
@@ -26481,7 +26491,7 @@
         <v>36</v>
       </c>
       <c r="H32" s="168" t="s">
-        <v>350</v>
+        <v>447</v>
       </c>
       <c r="I32" s="133" t="s">
         <v>157</v>
@@ -26492,7 +26502,7 @@
       </c>
       <c r="K32" s="126" t="str">
         <f>VLOOKUP(I32,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L32" s="117"/>
       <c r="M32" s="117"/>
@@ -26553,7 +26563,7 @@
     </row>
     <row r="33" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A33" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B33" s="119" t="s">
         <v>23</v>
@@ -26562,7 +26572,7 @@
         <v>24</v>
       </c>
       <c r="D33" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E33" s="145" t="s">
         <v>34</v>
@@ -26574,7 +26584,7 @@
         <v>36</v>
       </c>
       <c r="H33" s="168" t="s">
-        <v>351</v>
+        <v>448</v>
       </c>
       <c r="I33" s="133" t="s">
         <v>157</v>
@@ -26585,7 +26595,7 @@
       </c>
       <c r="K33" s="126" t="str">
         <f>VLOOKUP(I33,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L33" s="117"/>
       <c r="M33" s="117"/>
@@ -26646,7 +26656,7 @@
     </row>
     <row r="34" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A34" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B34" s="119" t="s">
         <v>23</v>
@@ -26655,7 +26665,7 @@
         <v>24</v>
       </c>
       <c r="D34" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E34" s="145" t="s">
         <v>34</v>
@@ -26667,7 +26677,7 @@
         <v>36</v>
       </c>
       <c r="H34" s="168" t="s">
-        <v>352</v>
+        <v>449</v>
       </c>
       <c r="I34" s="133" t="s">
         <v>216</v>
@@ -26678,7 +26688,7 @@
       </c>
       <c r="K34" s="126" t="str">
         <f>VLOOKUP(I34,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L34" s="117"/>
       <c r="M34" s="117"/>
@@ -26739,7 +26749,7 @@
     </row>
     <row r="35" spans="1:67" s="12" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B35" s="119" t="s">
         <v>23</v>
@@ -26748,7 +26758,7 @@
         <v>24</v>
       </c>
       <c r="D35" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E35" s="145" t="s">
         <v>34</v>
@@ -26760,7 +26770,7 @@
         <v>36</v>
       </c>
       <c r="H35" s="167" t="s">
-        <v>353</v>
+        <v>450</v>
       </c>
       <c r="I35" s="133" t="s">
         <v>216</v>
@@ -26771,7 +26781,7 @@
       </c>
       <c r="K35" s="126" t="str">
         <f>VLOOKUP(I35,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L35" s="117"/>
       <c r="M35" s="117"/>
@@ -26832,7 +26842,7 @@
     </row>
     <row r="36" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A36" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B36" s="119" t="s">
         <v>23</v>
@@ -26841,7 +26851,7 @@
         <v>24</v>
       </c>
       <c r="D36" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E36" s="145" t="s">
         <v>34</v>
@@ -26853,7 +26863,7 @@
         <v>36</v>
       </c>
       <c r="H36" s="167" t="s">
-        <v>354</v>
+        <v>451</v>
       </c>
       <c r="I36" s="133" t="s">
         <v>110</v>
@@ -26864,7 +26874,7 @@
       </c>
       <c r="K36" s="126" t="str">
         <f>VLOOKUP(I36,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L36" s="117"/>
       <c r="M36" s="117"/>
@@ -26925,7 +26935,7 @@
     </row>
     <row r="37" spans="1:67" s="12" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A37" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B37" s="119" t="s">
         <v>23</v>
@@ -26934,7 +26944,7 @@
         <v>24</v>
       </c>
       <c r="D37" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E37" s="145" t="s">
         <v>34</v>
@@ -26946,7 +26956,7 @@
         <v>36</v>
       </c>
       <c r="H37" s="167" t="s">
-        <v>355</v>
+        <v>452</v>
       </c>
       <c r="I37" s="133" t="s">
         <v>110</v>
@@ -26957,7 +26967,7 @@
       </c>
       <c r="K37" s="126" t="str">
         <f>VLOOKUP(I37,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L37" s="117"/>
       <c r="M37" s="117"/>
@@ -27016,9 +27026,9 @@
       <c r="BN37" s="117"/>
       <c r="BO37" s="117"/>
     </row>
-    <row r="38" spans="1:67" s="25" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:67" s="25" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A38" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B38" s="119" t="s">
         <v>23</v>
@@ -27027,7 +27037,7 @@
         <v>24</v>
       </c>
       <c r="D38" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E38" s="145" t="s">
         <v>34</v>
@@ -27039,7 +27049,7 @@
         <v>36</v>
       </c>
       <c r="H38" s="168" t="s">
-        <v>356</v>
+        <v>453</v>
       </c>
       <c r="I38" s="133" t="s">
         <v>110</v>
@@ -27050,7 +27060,7 @@
       </c>
       <c r="K38" s="126" t="str">
         <f>VLOOKUP(I38,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L38" s="117"/>
       <c r="M38" s="117"/>
@@ -27111,7 +27121,7 @@
     </row>
     <row r="39" spans="1:67" s="25" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B39" s="119" t="s">
         <v>23</v>
@@ -27120,7 +27130,7 @@
         <v>24</v>
       </c>
       <c r="D39" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E39" s="145" t="s">
         <v>34</v>
@@ -27132,7 +27142,7 @@
         <v>36</v>
       </c>
       <c r="H39" s="168" t="s">
-        <v>357</v>
+        <v>454</v>
       </c>
       <c r="I39" s="133" t="s">
         <v>172</v>
@@ -27143,7 +27153,7 @@
       </c>
       <c r="K39" s="126" t="str">
         <f>VLOOKUP(I39,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant, Staff users</v>
       </c>
       <c r="L39" s="117"/>
       <c r="M39" s="117"/>
@@ -27204,7 +27214,7 @@
     </row>
     <row r="40" spans="1:67" s="25" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A40" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B40" s="119" t="s">
         <v>23</v>
@@ -27213,7 +27223,7 @@
         <v>24</v>
       </c>
       <c r="D40" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E40" s="145" t="s">
         <v>34</v>
@@ -27225,7 +27235,7 @@
         <v>36</v>
       </c>
       <c r="H40" s="168" t="s">
-        <v>358</v>
+        <v>455</v>
       </c>
       <c r="I40" s="133" t="s">
         <v>172</v>
@@ -27236,7 +27246,7 @@
       </c>
       <c r="K40" s="126" t="str">
         <f>VLOOKUP(I40,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant, Staff users</v>
       </c>
       <c r="L40" s="117"/>
       <c r="M40" s="117"/>
@@ -27297,7 +27307,7 @@
     </row>
     <row r="41" spans="1:67" s="25" customFormat="1" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="132" t="s">
-        <v>22</v>
+        <v>398</v>
       </c>
       <c r="B41" s="119" t="s">
         <v>23</v>
@@ -27306,7 +27316,7 @@
         <v>24</v>
       </c>
       <c r="D41" s="118" t="s">
-        <v>33</v>
+        <v>407</v>
       </c>
       <c r="E41" s="145" t="s">
         <v>34</v>
@@ -27318,7 +27328,7 @@
         <v>36</v>
       </c>
       <c r="H41" s="168" t="s">
-        <v>359</v>
+        <v>456</v>
       </c>
       <c r="I41" s="133" t="s">
         <v>110</v>
@@ -27329,7 +27339,7 @@
       </c>
       <c r="K41" s="126" t="str">
         <f>VLOOKUP(I41,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L41" s="117"/>
       <c r="M41" s="117"/>
@@ -27390,7 +27400,7 @@
     </row>
     <row r="42" spans="1:67" s="25" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B42" s="121" t="s">
         <v>38</v>
@@ -27399,7 +27409,7 @@
         <v>39</v>
       </c>
       <c r="D42" s="120" t="s">
-        <v>40</v>
+        <v>408</v>
       </c>
       <c r="E42" s="146" t="s">
         <v>41</v>
@@ -27411,7 +27421,7 @@
         <v>43</v>
       </c>
       <c r="H42" s="169" t="s">
-        <v>360</v>
+        <v>457</v>
       </c>
       <c r="I42" s="135" t="s">
         <v>110</v>
@@ -27422,7 +27432,7 @@
       </c>
       <c r="K42" s="126" t="str">
         <f>VLOOKUP(I42,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant users, Staff users, Secondary users</v>
       </c>
       <c r="L42" s="117"/>
       <c r="M42" s="117"/>
@@ -27483,7 +27493,7 @@
     </row>
     <row r="43" spans="1:67" s="25" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A43" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B43" s="121" t="s">
         <v>38</v>
@@ -27492,7 +27502,7 @@
         <v>39</v>
       </c>
       <c r="D43" s="120" t="s">
-        <v>40</v>
+        <v>408</v>
       </c>
       <c r="E43" s="146" t="s">
         <v>41</v>
@@ -27504,7 +27514,7 @@
         <v>43</v>
       </c>
       <c r="H43" s="170" t="s">
-        <v>361</v>
+        <v>458</v>
       </c>
       <c r="I43" s="135" t="s">
         <v>157</v>
@@ -27515,7 +27525,7 @@
       </c>
       <c r="K43" s="126" t="str">
         <f>VLOOKUP(I43,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L43" s="117"/>
       <c r="M43" s="117"/>
@@ -27576,7 +27586,7 @@
     </row>
     <row r="44" spans="1:67" s="25" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B44" s="121" t="s">
         <v>38</v>
@@ -27585,7 +27595,7 @@
         <v>39</v>
       </c>
       <c r="D44" s="120" t="s">
-        <v>40</v>
+        <v>408</v>
       </c>
       <c r="E44" s="146" t="s">
         <v>41</v>
@@ -27597,7 +27607,7 @@
         <v>43</v>
       </c>
       <c r="H44" s="169" t="s">
-        <v>362</v>
+        <v>459</v>
       </c>
       <c r="I44" s="135" t="s">
         <v>157</v>
@@ -27608,7 +27618,7 @@
       </c>
       <c r="K44" s="126" t="str">
         <f>VLOOKUP(I44,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L44" s="117"/>
       <c r="M44" s="117"/>
@@ -27669,7 +27679,7 @@
     </row>
     <row r="45" spans="1:67" s="25" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A45" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B45" s="121" t="s">
         <v>38</v>
@@ -27678,7 +27688,7 @@
         <v>39</v>
       </c>
       <c r="D45" s="120" t="s">
-        <v>40</v>
+        <v>408</v>
       </c>
       <c r="E45" s="146" t="s">
         <v>41</v>
@@ -27690,7 +27700,7 @@
         <v>43</v>
       </c>
       <c r="H45" s="169" t="s">
-        <v>363</v>
+        <v>460</v>
       </c>
       <c r="I45" s="135" t="s">
         <v>157</v>
@@ -27701,7 +27711,7 @@
       </c>
       <c r="K45" s="126" t="str">
         <f>VLOOKUP(I45,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Participant users, Staff users, Tertiary users</v>
       </c>
       <c r="L45" s="117"/>
       <c r="M45" s="117"/>
@@ -27762,7 +27772,7 @@
     </row>
     <row r="46" spans="1:67" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B46" s="121" t="s">
         <v>38</v>
@@ -27771,7 +27781,7 @@
         <v>39</v>
       </c>
       <c r="D46" s="120" t="s">
-        <v>273</v>
+        <v>409</v>
       </c>
       <c r="E46" s="146" t="s">
         <v>45</v>
@@ -27783,7 +27793,7 @@
         <v>47</v>
       </c>
       <c r="H46" s="170" t="s">
-        <v>364</v>
+        <v>461</v>
       </c>
       <c r="I46" s="135" t="s">
         <v>186</v>
@@ -27794,7 +27804,7 @@
       </c>
       <c r="K46" s="126" t="str">
         <f>VLOOKUP(I46,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L46" s="117"/>
       <c r="M46" s="117"/>
@@ -27855,7 +27865,7 @@
     </row>
     <row r="47" spans="1:67" s="34" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B47" s="121" t="s">
         <v>38</v>
@@ -27864,7 +27874,7 @@
         <v>39</v>
       </c>
       <c r="D47" s="120" t="s">
-        <v>273</v>
+        <v>409</v>
       </c>
       <c r="E47" s="146" t="s">
         <v>45</v>
@@ -27876,7 +27886,7 @@
         <v>47</v>
       </c>
       <c r="H47" s="169" t="s">
-        <v>365</v>
+        <v>462</v>
       </c>
       <c r="I47" s="135" t="s">
         <v>186</v>
@@ -27887,7 +27897,7 @@
       </c>
       <c r="K47" s="126" t="str">
         <f>VLOOKUP(I47,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L47" s="117"/>
       <c r="M47" s="117"/>
@@ -27948,7 +27958,7 @@
     </row>
     <row r="48" spans="1:67" s="34" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B48" s="121" t="s">
         <v>38</v>
@@ -27957,7 +27967,7 @@
         <v>39</v>
       </c>
       <c r="D48" s="120" t="s">
-        <v>273</v>
+        <v>409</v>
       </c>
       <c r="E48" s="146" t="s">
         <v>45</v>
@@ -27969,7 +27979,7 @@
         <v>47</v>
       </c>
       <c r="H48" s="169" t="s">
-        <v>366</v>
+        <v>463</v>
       </c>
       <c r="I48" s="135" t="s">
         <v>186</v>
@@ -27980,7 +27990,7 @@
       </c>
       <c r="K48" s="126" t="str">
         <f>VLOOKUP(I48,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L48" s="117"/>
       <c r="M48" s="117"/>
@@ -28041,7 +28051,7 @@
     </row>
     <row r="49" spans="1:67" s="34" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A49" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B49" s="121" t="s">
         <v>38</v>
@@ -28050,7 +28060,7 @@
         <v>39</v>
       </c>
       <c r="D49" s="120" t="s">
-        <v>48</v>
+        <v>410</v>
       </c>
       <c r="E49" s="146" t="s">
         <v>49</v>
@@ -28062,7 +28072,7 @@
         <v>51</v>
       </c>
       <c r="H49" s="170" t="s">
-        <v>367</v>
+        <v>464</v>
       </c>
       <c r="I49" s="135" t="s">
         <v>186</v>
@@ -28073,7 +28083,7 @@
       </c>
       <c r="K49" s="126" t="str">
         <f>VLOOKUP(I49,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L49" s="117"/>
       <c r="M49" s="117"/>
@@ -28134,7 +28144,7 @@
     </row>
     <row r="50" spans="1:67" s="34" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A50" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B50" s="121" t="s">
         <v>38</v>
@@ -28143,7 +28153,7 @@
         <v>39</v>
       </c>
       <c r="D50" s="120" t="s">
-        <v>48</v>
+        <v>410</v>
       </c>
       <c r="E50" s="146" t="s">
         <v>49</v>
@@ -28155,7 +28165,7 @@
         <v>51</v>
       </c>
       <c r="H50" s="170" t="s">
-        <v>368</v>
+        <v>465</v>
       </c>
       <c r="I50" s="135" t="s">
         <v>186</v>
@@ -28166,7 +28176,7 @@
       </c>
       <c r="K50" s="126" t="str">
         <f>VLOOKUP(I50,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L50" s="117"/>
       <c r="M50" s="117"/>
@@ -28227,7 +28237,7 @@
     </row>
     <row r="51" spans="1:67" s="34" customFormat="1" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B51" s="121" t="s">
         <v>38</v>
@@ -28236,7 +28246,7 @@
         <v>39</v>
       </c>
       <c r="D51" s="120" t="s">
-        <v>52</v>
+        <v>411</v>
       </c>
       <c r="E51" s="146" t="s">
         <v>53</v>
@@ -28248,7 +28258,7 @@
         <v>55</v>
       </c>
       <c r="H51" s="170" t="s">
-        <v>369</v>
+        <v>466</v>
       </c>
       <c r="I51" s="135" t="s">
         <v>186</v>
@@ -28259,7 +28269,7 @@
       </c>
       <c r="K51" s="126" t="str">
         <f>VLOOKUP(I51,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L51" s="117"/>
       <c r="M51" s="117"/>
@@ -28320,7 +28330,7 @@
     </row>
     <row r="52" spans="1:67" s="39" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="134" t="s">
-        <v>37</v>
+        <v>399</v>
       </c>
       <c r="B52" s="121" t="s">
         <v>38</v>
@@ -28329,7 +28339,7 @@
         <v>39</v>
       </c>
       <c r="D52" s="120" t="s">
-        <v>52</v>
+        <v>411</v>
       </c>
       <c r="E52" s="146" t="s">
         <v>53</v>
@@ -28341,7 +28351,7 @@
         <v>55</v>
       </c>
       <c r="H52" s="170" t="s">
-        <v>370</v>
+        <v>467</v>
       </c>
       <c r="I52" s="135" t="s">
         <v>186</v>
@@ -28352,7 +28362,7 @@
       </c>
       <c r="K52" s="126" t="str">
         <f>VLOOKUP(I52,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Clinical Staff, Operational Staff</v>
+        <v>Participant, Staff users, Tertiary users</v>
       </c>
       <c r="L52" s="117"/>
       <c r="M52" s="117"/>
@@ -28413,7 +28423,7 @@
     </row>
     <row r="53" spans="1:67" s="39" customFormat="1" ht="98" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="136" t="s">
-        <v>56</v>
+        <v>400</v>
       </c>
       <c r="B53" s="123" t="s">
         <v>57</v>
@@ -28422,7 +28432,7 @@
         <v>58</v>
       </c>
       <c r="D53" s="122" t="s">
-        <v>59</v>
+        <v>412</v>
       </c>
       <c r="E53" s="147" t="s">
         <v>60</v>
@@ -28434,7 +28444,7 @@
         <v>62</v>
       </c>
       <c r="H53" s="171" t="s">
-        <v>447</v>
+        <v>468</v>
       </c>
       <c r="I53" s="137" t="s">
         <v>175</v>
@@ -28445,7 +28455,7 @@
       </c>
       <c r="K53" s="126" t="str">
         <f>VLOOKUP(I53,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L53" s="117"/>
       <c r="M53" s="117"/>
@@ -28506,7 +28516,7 @@
     </row>
     <row r="54" spans="1:67" s="39" customFormat="1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="136" t="s">
-        <v>56</v>
+        <v>400</v>
       </c>
       <c r="B54" s="123" t="s">
         <v>57</v>
@@ -28515,7 +28525,7 @@
         <v>58</v>
       </c>
       <c r="D54" s="122" t="s">
-        <v>59</v>
+        <v>412</v>
       </c>
       <c r="E54" s="147" t="s">
         <v>60</v>
@@ -28527,7 +28537,7 @@
         <v>62</v>
       </c>
       <c r="H54" s="176" t="s">
-        <v>448</v>
+        <v>469</v>
       </c>
       <c r="I54" s="137" t="s">
         <v>175</v>
@@ -28538,7 +28548,7 @@
       </c>
       <c r="K54" s="126" t="str">
         <f>VLOOKUP(I54,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L54" s="117"/>
       <c r="M54" s="117"/>
@@ -28599,7 +28609,7 @@
     </row>
     <row r="55" spans="1:67" s="39" customFormat="1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="136" t="s">
-        <v>56</v>
+        <v>400</v>
       </c>
       <c r="B55" s="123" t="s">
         <v>57</v>
@@ -28608,7 +28618,7 @@
         <v>58</v>
       </c>
       <c r="D55" s="122" t="s">
-        <v>63</v>
+        <v>413</v>
       </c>
       <c r="E55" s="147" t="s">
         <v>315</v>
@@ -28620,7 +28630,7 @@
         <v>66</v>
       </c>
       <c r="H55" s="171" t="s">
-        <v>449</v>
+        <v>470</v>
       </c>
       <c r="I55" s="137" t="s">
         <v>175</v>
@@ -28631,7 +28641,7 @@
       </c>
       <c r="K55" s="126" t="str">
         <f>VLOOKUP(I55,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L55" s="117"/>
       <c r="M55" s="117"/>
@@ -28692,7 +28702,7 @@
     </row>
     <row r="56" spans="1:67" s="39" customFormat="1" ht="106" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="136" t="s">
-        <v>56</v>
+        <v>400</v>
       </c>
       <c r="B56" s="123" t="s">
         <v>57</v>
@@ -28701,7 +28711,7 @@
         <v>58</v>
       </c>
       <c r="D56" s="122" t="s">
-        <v>63</v>
+        <v>413</v>
       </c>
       <c r="E56" s="147" t="s">
         <v>315</v>
@@ -28713,7 +28723,7 @@
         <v>66</v>
       </c>
       <c r="H56" s="171" t="s">
-        <v>450</v>
+        <v>471</v>
       </c>
       <c r="I56" s="137" t="s">
         <v>175</v>
@@ -28724,7 +28734,7 @@
       </c>
       <c r="K56" s="126" t="str">
         <f>VLOOKUP(I56,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L56" s="117"/>
       <c r="M56" s="117"/>
@@ -28785,7 +28795,7 @@
     </row>
     <row r="57" spans="1:67" s="6" customFormat="1" ht="102" x14ac:dyDescent="0.2">
       <c r="A57" s="136" t="s">
-        <v>56</v>
+        <v>400</v>
       </c>
       <c r="B57" s="123" t="s">
         <v>57</v>
@@ -28794,7 +28804,7 @@
         <v>58</v>
       </c>
       <c r="D57" s="122" t="s">
-        <v>63</v>
+        <v>413</v>
       </c>
       <c r="E57" s="147" t="s">
         <v>315</v>
@@ -28806,7 +28816,7 @@
         <v>66</v>
       </c>
       <c r="H57" s="171" t="s">
-        <v>451</v>
+        <v>472</v>
       </c>
       <c r="I57" s="137" t="s">
         <v>216</v>
@@ -28817,7 +28827,7 @@
       </c>
       <c r="K57" s="126" t="str">
         <f>VLOOKUP(I57,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant, Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L57" s="117"/>
       <c r="M57" s="117"/>
@@ -28878,7 +28888,7 @@
     </row>
     <row r="58" spans="1:67" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A58" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B58" s="125" t="s">
         <v>68</v>
@@ -28887,7 +28897,7 @@
         <v>69</v>
       </c>
       <c r="D58" s="124" t="s">
-        <v>300</v>
+        <v>414</v>
       </c>
       <c r="E58" s="148" t="s">
         <v>71</v>
@@ -28899,7 +28909,7 @@
         <v>73</v>
       </c>
       <c r="H58" s="172" t="s">
-        <v>372</v>
+        <v>473</v>
       </c>
       <c r="I58" s="138" t="s">
         <v>87</v>
@@ -28910,7 +28920,7 @@
       </c>
       <c r="K58" s="126" t="str">
         <f>VLOOKUP(I58,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L58" s="117"/>
       <c r="M58" s="117"/>
@@ -28971,7 +28981,7 @@
     </row>
     <row r="59" spans="1:67" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A59" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B59" s="125" t="s">
         <v>68</v>
@@ -28980,7 +28990,7 @@
         <v>69</v>
       </c>
       <c r="D59" s="124" t="s">
-        <v>300</v>
+        <v>414</v>
       </c>
       <c r="E59" s="148" t="s">
         <v>71</v>
@@ -28992,7 +29002,7 @@
         <v>73</v>
       </c>
       <c r="H59" s="173" t="s">
-        <v>373</v>
+        <v>474</v>
       </c>
       <c r="I59" s="138" t="s">
         <v>175</v>
@@ -29003,7 +29013,7 @@
       </c>
       <c r="K59" s="126" t="str">
         <f>VLOOKUP(I59,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L59" s="117"/>
       <c r="M59" s="117"/>
@@ -29064,7 +29074,7 @@
     </row>
     <row r="60" spans="1:67" s="6" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A60" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B60" s="125" t="s">
         <v>68</v>
@@ -29073,7 +29083,7 @@
         <v>69</v>
       </c>
       <c r="D60" s="124" t="s">
-        <v>300</v>
+        <v>414</v>
       </c>
       <c r="E60" s="148" t="s">
         <v>71</v>
@@ -29085,7 +29095,7 @@
         <v>73</v>
       </c>
       <c r="H60" s="172" t="s">
-        <v>374</v>
+        <v>475</v>
       </c>
       <c r="I60" s="138" t="s">
         <v>87</v>
@@ -29096,7 +29106,7 @@
       </c>
       <c r="K60" s="126" t="str">
         <f>VLOOKUP(I60,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L60" s="117"/>
       <c r="M60" s="117"/>
@@ -29157,7 +29167,7 @@
     </row>
     <row r="61" spans="1:67" s="6" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B61" s="125" t="s">
         <v>68</v>
@@ -29166,7 +29176,7 @@
         <v>69</v>
       </c>
       <c r="D61" s="124" t="s">
-        <v>452</v>
+        <v>415</v>
       </c>
       <c r="E61" s="148" t="s">
         <v>75</v>
@@ -29178,7 +29188,7 @@
         <v>77</v>
       </c>
       <c r="H61" s="172" t="s">
-        <v>375</v>
+        <v>476</v>
       </c>
       <c r="I61" s="138" t="s">
         <v>87</v>
@@ -29189,7 +29199,7 @@
       </c>
       <c r="K61" s="126" t="str">
         <f>VLOOKUP(I61,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L61" s="117"/>
       <c r="M61" s="117"/>
@@ -29250,7 +29260,7 @@
     </row>
     <row r="62" spans="1:67" ht="136" x14ac:dyDescent="0.2">
       <c r="A62" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B62" s="125" t="s">
         <v>68</v>
@@ -29259,7 +29269,7 @@
         <v>69</v>
       </c>
       <c r="D62" s="124" t="s">
-        <v>452</v>
+        <v>415</v>
       </c>
       <c r="E62" s="148" t="s">
         <v>75</v>
@@ -29271,7 +29281,7 @@
         <v>77</v>
       </c>
       <c r="H62" s="172" t="s">
-        <v>376</v>
+        <v>477</v>
       </c>
       <c r="I62" s="138" t="s">
         <v>87</v>
@@ -29282,7 +29292,7 @@
       </c>
       <c r="K62" s="126" t="str">
         <f>VLOOKUP(I62,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L62" s="117"/>
       <c r="M62" s="117"/>
@@ -29343,7 +29353,7 @@
     </row>
     <row r="63" spans="1:67" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B63" s="125" t="s">
         <v>68</v>
@@ -29352,7 +29362,7 @@
         <v>69</v>
       </c>
       <c r="D63" s="124" t="s">
-        <v>78</v>
+        <v>416</v>
       </c>
       <c r="E63" s="148" t="s">
         <v>79</v>
@@ -29364,7 +29374,7 @@
         <v>81</v>
       </c>
       <c r="H63" s="173" t="s">
-        <v>377</v>
+        <v>478</v>
       </c>
       <c r="I63" s="138" t="s">
         <v>122</v>
@@ -29375,7 +29385,7 @@
       </c>
       <c r="K63" s="126" t="str">
         <f>VLOOKUP(I63,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Secondary users</v>
       </c>
       <c r="L63" s="117"/>
       <c r="M63" s="117"/>
@@ -29436,7 +29446,7 @@
     </row>
     <row r="64" spans="1:67" ht="170" x14ac:dyDescent="0.2">
       <c r="A64" s="301" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B64" s="125" t="s">
         <v>68</v>
@@ -29445,7 +29455,7 @@
         <v>69</v>
       </c>
       <c r="D64" s="124" t="s">
-        <v>78</v>
+        <v>416</v>
       </c>
       <c r="E64" s="148" t="s">
         <v>79</v>
@@ -29457,7 +29467,7 @@
         <v>81</v>
       </c>
       <c r="H64" s="172" t="s">
-        <v>378</v>
+        <v>479</v>
       </c>
       <c r="I64" s="138" t="s">
         <v>87</v>
@@ -29468,7 +29478,7 @@
       </c>
       <c r="K64" s="126" t="str">
         <f>VLOOKUP(I64,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L64" s="117"/>
       <c r="M64" s="117"/>
@@ -29529,7 +29539,7 @@
     </row>
     <row r="65" spans="1:67" ht="170" x14ac:dyDescent="0.2">
       <c r="A65" s="302" t="s">
-        <v>67</v>
+        <v>401</v>
       </c>
       <c r="B65" s="139" t="s">
         <v>68</v>
@@ -29538,7 +29548,7 @@
         <v>69</v>
       </c>
       <c r="D65" s="140" t="s">
-        <v>78</v>
+        <v>416</v>
       </c>
       <c r="E65" s="149" t="s">
         <v>79</v>
@@ -29550,7 +29560,7 @@
         <v>81</v>
       </c>
       <c r="H65" s="174" t="s">
-        <v>379</v>
+        <v>480</v>
       </c>
       <c r="I65" s="141" t="s">
         <v>87</v>
@@ -29561,7 +29571,7 @@
       </c>
       <c r="K65" s="126" t="str">
         <f>VLOOKUP(I65,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Operational Staff</v>
+        <v>Staff users, Secondary users</v>
       </c>
       <c r="L65" s="117"/>
       <c r="M65" s="117"/>
@@ -29969,7 +29979,7 @@
     <row r="72" spans="1:67" ht="16" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:67" ht="16" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:J65" xr:uid="{B771BD26-5CB2-F242-A0FA-A4D8589272A0}"/>
+  <autoFilter ref="A1:K65" xr:uid="{B771BD26-5CB2-F242-A0FA-A4D8589272A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -29980,8 +29990,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8096783-64B1-C547-94F3-04D3BE1EF5B1}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29999,7 +30009,7 @@
         <v>83</v>
       </c>
       <c r="C1" s="337" t="s">
-        <v>454</v>
+        <v>388</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
@@ -30007,10 +30017,10 @@
         <v>87</v>
       </c>
       <c r="B2" s="178" t="s">
-        <v>444</v>
+        <v>386</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -30021,7 +30031,7 @@
         <v>106</v>
       </c>
       <c r="C3" t="s">
-        <v>456</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
@@ -30032,7 +30042,7 @@
         <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -30043,7 +30053,7 @@
         <v>123</v>
       </c>
       <c r="C5" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
@@ -30054,7 +30064,7 @@
         <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -30065,7 +30075,7 @@
         <v>132</v>
       </c>
       <c r="C7" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
@@ -30076,7 +30086,7 @@
         <v>138</v>
       </c>
       <c r="C8" t="s">
-        <v>455</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -30087,7 +30097,7 @@
         <v>142</v>
       </c>
       <c r="C9" t="s">
-        <v>455</v>
+        <v>392</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -30098,7 +30108,7 @@
         <v>150</v>
       </c>
       <c r="C10" t="s">
-        <v>457</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
@@ -30109,7 +30119,7 @@
         <v>158</v>
       </c>
       <c r="C11" t="s">
-        <v>457</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="52" thickBot="1" x14ac:dyDescent="0.25">
@@ -30120,7 +30130,7 @@
         <v>173</v>
       </c>
       <c r="C12" t="s">
-        <v>457</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="154" thickBot="1" x14ac:dyDescent="0.25">
@@ -30131,7 +30141,7 @@
         <v>176</v>
       </c>
       <c r="C13" t="s">
-        <v>455</v>
+        <v>394</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
@@ -30142,7 +30152,7 @@
         <v>187</v>
       </c>
       <c r="C14" t="s">
-        <v>453</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -30172,7 +30182,7 @@
         <v>82</v>
       </c>
       <c r="B1" s="184" t="s">
-        <v>443</v>
+        <v>385</v>
       </c>
       <c r="C1" s="186" t="s">
         <v>84</v>
@@ -30192,7 +30202,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="192" t="s">
-        <v>381</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30200,7 +30210,7 @@
       <c r="B3" s="194"/>
       <c r="C3" s="195"/>
       <c r="D3" s="196" t="s">
-        <v>406</v>
+        <v>348</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30214,7 +30224,7 @@
         <v>29</v>
       </c>
       <c r="D4" s="200" t="s">
-        <v>383</v>
+        <v>325</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30222,7 +30232,7 @@
       <c r="B5" s="202"/>
       <c r="C5" s="203"/>
       <c r="D5" s="204" t="s">
-        <v>384</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30230,7 +30240,7 @@
       <c r="B6" s="202"/>
       <c r="C6" s="203"/>
       <c r="D6" s="204" t="s">
-        <v>386</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30238,7 +30248,7 @@
       <c r="B7" s="202"/>
       <c r="C7" s="203"/>
       <c r="D7" s="204" t="s">
-        <v>440</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30248,7 +30258,7 @@
         <v>33</v>
       </c>
       <c r="D8" s="204" t="s">
-        <v>382</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30256,7 +30266,7 @@
       <c r="B9" s="202"/>
       <c r="C9" s="203"/>
       <c r="D9" s="204" t="s">
-        <v>385</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30264,7 +30274,7 @@
       <c r="B10" s="202"/>
       <c r="C10" s="203"/>
       <c r="D10" s="204" t="s">
-        <v>387</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30272,7 +30282,7 @@
       <c r="B11" s="202"/>
       <c r="C11" s="203"/>
       <c r="D11" s="204" t="s">
-        <v>388</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30282,7 +30292,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="204" t="s">
-        <v>404</v>
+        <v>346</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="102" customHeight="1" x14ac:dyDescent="0.2">
@@ -30290,13 +30300,13 @@
         <v>87</v>
       </c>
       <c r="B13" s="210" t="s">
-        <v>444</v>
+        <v>386</v>
       </c>
       <c r="C13" s="211" t="s">
         <v>10</v>
       </c>
       <c r="D13" s="212" t="s">
-        <v>395</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30304,7 +30314,7 @@
       <c r="B14" s="214"/>
       <c r="C14" s="215"/>
       <c r="D14" s="216" t="s">
-        <v>441</v>
+        <v>383</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30314,7 +30324,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="216" t="s">
-        <v>389</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30324,7 +30334,7 @@
         <v>300</v>
       </c>
       <c r="D16" s="216" t="s">
-        <v>418</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30332,7 +30342,7 @@
       <c r="B17" s="214"/>
       <c r="C17" s="215"/>
       <c r="D17" s="216" t="s">
-        <v>423</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30342,7 +30352,7 @@
         <v>74</v>
       </c>
       <c r="D18" s="216" t="s">
-        <v>398</v>
+        <v>340</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30350,7 +30360,7 @@
       <c r="B19" s="214"/>
       <c r="C19" s="215"/>
       <c r="D19" s="216" t="s">
-        <v>428</v>
+        <v>370</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30360,7 +30370,7 @@
         <v>78</v>
       </c>
       <c r="D20" s="216" t="s">
-        <v>399</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30368,7 +30378,7 @@
       <c r="B21" s="214"/>
       <c r="C21" s="215"/>
       <c r="D21" s="216" t="s">
-        <v>407</v>
+        <v>349</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="69" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -30382,7 +30392,7 @@
         <v>78</v>
       </c>
       <c r="D22" s="208" t="s">
-        <v>415</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -30396,7 +30406,7 @@
         <v>14</v>
       </c>
       <c r="D23" s="220" t="s">
-        <v>411</v>
+        <v>353</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30404,7 +30414,7 @@
       <c r="B24" s="222"/>
       <c r="C24" s="223"/>
       <c r="D24" s="224" t="s">
-        <v>412</v>
+        <v>354</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -30418,7 +30428,7 @@
         <v>18</v>
       </c>
       <c r="D25" s="228" t="s">
-        <v>402</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30426,7 +30436,7 @@
       <c r="B26" s="230"/>
       <c r="C26" s="231"/>
       <c r="D26" s="232" t="s">
-        <v>403</v>
+        <v>345</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30434,7 +30444,7 @@
       <c r="B27" s="230"/>
       <c r="C27" s="231"/>
       <c r="D27" s="232" t="s">
-        <v>437</v>
+        <v>379</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30442,7 +30452,7 @@
       <c r="B28" s="230"/>
       <c r="C28" s="231"/>
       <c r="D28" s="232" t="s">
-        <v>438</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="68" x14ac:dyDescent="0.2">
@@ -30456,7 +30466,7 @@
         <v>18</v>
       </c>
       <c r="D29" s="236" t="s">
-        <v>400</v>
+        <v>342</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30464,7 +30474,7 @@
       <c r="B30" s="238"/>
       <c r="C30" s="239"/>
       <c r="D30" s="240" t="s">
-        <v>430</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30478,7 +30488,7 @@
         <v>18</v>
       </c>
       <c r="D31" s="244" t="s">
-        <v>429</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30488,7 +30498,7 @@
         <v>25</v>
       </c>
       <c r="D32" s="248" t="s">
-        <v>391</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30496,7 +30506,7 @@
       <c r="B33" s="246"/>
       <c r="C33" s="247"/>
       <c r="D33" s="248" t="s">
-        <v>397</v>
+        <v>339</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30504,7 +30514,7 @@
       <c r="B34" s="246"/>
       <c r="C34" s="247"/>
       <c r="D34" s="248" t="s">
-        <v>434</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30512,7 +30522,7 @@
       <c r="B35" s="246"/>
       <c r="C35" s="247"/>
       <c r="D35" s="248" t="s">
-        <v>435</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30520,21 +30530,21 @@
       <c r="B36" s="250"/>
       <c r="C36" s="251"/>
       <c r="D36" s="252" t="s">
-        <v>439</v>
+        <v>381</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="185" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="B37" s="93" t="s">
-        <v>445</v>
+        <v>387</v>
       </c>
       <c r="C37" s="185" t="s">
         <v>25</v>
       </c>
       <c r="D37" s="188" t="s">
-        <v>390</v>
+        <v>332</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="66" customHeight="1" x14ac:dyDescent="0.2">
@@ -30548,7 +30558,7 @@
         <v>29</v>
       </c>
       <c r="D38" s="256" t="s">
-        <v>436</v>
+        <v>378</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30558,7 +30568,7 @@
         <v>33</v>
       </c>
       <c r="D39" s="260" t="s">
-        <v>416</v>
+        <v>358</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30566,7 +30576,7 @@
       <c r="B40" s="258"/>
       <c r="C40" s="259"/>
       <c r="D40" s="260" t="s">
-        <v>419</v>
+        <v>361</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30576,21 +30586,21 @@
         <v>63</v>
       </c>
       <c r="D41" s="264" t="s">
-        <v>393</v>
+        <v>335</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="185" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="B42" s="93" t="s">
-        <v>445</v>
+        <v>387</v>
       </c>
       <c r="C42" s="185" t="s">
         <v>14</v>
       </c>
       <c r="D42" s="188" t="s">
-        <v>396</v>
+        <v>338</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -30604,7 +30614,7 @@
         <v>33</v>
       </c>
       <c r="D43" s="268" t="s">
-        <v>380</v>
+        <v>322</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30612,7 +30622,7 @@
       <c r="B44" s="270"/>
       <c r="C44" s="271"/>
       <c r="D44" s="272" t="s">
-        <v>420</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30620,7 +30630,7 @@
       <c r="B45" s="270"/>
       <c r="C45" s="271"/>
       <c r="D45" s="272" t="s">
-        <v>424</v>
+        <v>366</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30628,7 +30638,7 @@
       <c r="B46" s="270"/>
       <c r="C46" s="271"/>
       <c r="D46" s="272" t="s">
-        <v>426</v>
+        <v>368</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30638,7 +30648,7 @@
         <v>40</v>
       </c>
       <c r="D47" s="272" t="s">
-        <v>417</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30646,7 +30656,7 @@
       <c r="B48" s="270"/>
       <c r="C48" s="271"/>
       <c r="D48" s="272" t="s">
-        <v>425</v>
+        <v>367</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30654,7 +30664,7 @@
       <c r="B49" s="270"/>
       <c r="C49" s="271"/>
       <c r="D49" s="272" t="s">
-        <v>427</v>
+        <v>369</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="51" x14ac:dyDescent="0.2">
@@ -30668,7 +30678,7 @@
         <v>33</v>
       </c>
       <c r="D50" s="276" t="s">
-        <v>405</v>
+        <v>347</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30676,7 +30686,7 @@
       <c r="B51" s="278"/>
       <c r="C51" s="279"/>
       <c r="D51" s="280" t="s">
-        <v>414</v>
+        <v>356</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="137.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -30690,7 +30700,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="284" t="s">
-        <v>413</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -30698,7 +30708,7 @@
       <c r="B53" s="286"/>
       <c r="C53" s="287"/>
       <c r="D53" s="288" t="s">
-        <v>421</v>
+        <v>363</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30708,7 +30718,7 @@
         <v>59</v>
       </c>
       <c r="D54" s="288" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30716,7 +30726,7 @@
       <c r="B55" s="286"/>
       <c r="C55" s="287"/>
       <c r="D55" s="288" t="s">
-        <v>401</v>
+        <v>343</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30726,7 +30736,7 @@
         <v>63</v>
       </c>
       <c r="D56" s="288" t="s">
-        <v>392</v>
+        <v>334</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30734,7 +30744,7 @@
       <c r="B57" s="286"/>
       <c r="C57" s="287"/>
       <c r="D57" s="288" t="s">
-        <v>442</v>
+        <v>384</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30744,7 +30754,7 @@
         <v>300</v>
       </c>
       <c r="D58" s="288" t="s">
-        <v>422</v>
+        <v>364</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -30758,7 +30768,7 @@
         <v>273</v>
       </c>
       <c r="D59" s="292" t="s">
-        <v>394</v>
+        <v>336</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30766,7 +30776,7 @@
       <c r="B60" s="294"/>
       <c r="C60" s="295"/>
       <c r="D60" s="296" t="s">
-        <v>408</v>
+        <v>350</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30774,7 +30784,7 @@
       <c r="B61" s="294"/>
       <c r="C61" s="295"/>
       <c r="D61" s="296" t="s">
-        <v>433</v>
+        <v>375</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30784,7 +30794,7 @@
         <v>48</v>
       </c>
       <c r="D62" s="296" t="s">
-        <v>409</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30792,7 +30802,7 @@
       <c r="B63" s="294"/>
       <c r="C63" s="295"/>
       <c r="D63" s="296" t="s">
-        <v>410</v>
+        <v>352</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -30802,7 +30812,7 @@
         <v>52</v>
       </c>
       <c r="D64" s="296" t="s">
-        <v>431</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" thickBot="1" x14ac:dyDescent="0.25">
@@ -30810,7 +30820,7 @@
       <c r="B65" s="298"/>
       <c r="C65" s="299"/>
       <c r="D65" s="300" t="s">
-        <v>432</v>
+        <v>374</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated to include data domains
</commit_message>
<xml_diff>
--- a/data/BusinessCapabilitiesv0.1.xlsx
+++ b/data/BusinessCapabilitiesv0.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leegath/LAG/Fathomatics/code/nhse/capabilitygenerator/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF8654-F7D9-E742-8A79-6F8A41ED8535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75EBBB9C-B0CC-8342-BC64-A21C9DE7480F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="26580" activeTab="3" xr2:uid="{FB9E69F6-520F-B448-8326-5E7FF50D6D4B}"/>
+    <workbookView xWindow="34120" yWindow="500" windowWidth="34140" windowHeight="26580" activeTab="3" xr2:uid="{FB9E69F6-520F-B448-8326-5E7FF50D6D4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Capability Map" sheetId="10" r:id="rId1"/>
@@ -404,7 +404,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1500" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1533" uniqueCount="505">
   <si>
     <t>Value Stream Stage</t>
   </si>
@@ -2541,6 +2541,78 @@
       </rPr>
       <t>: Conduct investigations and take corrective actions.</t>
     </r>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Audit</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Root Entity</t>
+  </si>
+  <si>
+    <t>Appointment</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>Capacity/Demand</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Allocation</t>
+  </si>
+  <si>
+    <t>Cohorting as a Service manages cohort definitions and informs Cohort Manager when a participant changes in their eligibility status</t>
+  </si>
+  <si>
+    <t>Staff users</t>
+  </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>Clinical, Diagnostic</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>Provisional slot, Provisional appointment request</t>
+  </si>
+  <si>
+    <t>Slot</t>
+  </si>
+  <si>
+    <t>Eligible Participant</t>
+  </si>
+  <si>
+    <t>Invitable Participant</t>
+  </si>
+  <si>
+    <t>Letter, Email, Text Message</t>
+  </si>
+  <si>
+    <t>Participant, Episode</t>
+  </si>
+  <si>
+    <t>Requirement for slot, Encounter</t>
+  </si>
+  <si>
+    <t>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</t>
   </si>
 </sst>
 </file>
@@ -3133,7 +3205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="339">
+  <cellXfs count="345">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3967,30 +4039,8 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -4045,13 +4095,37 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4069,8 +4143,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11791,13 +11879,13 @@
       </c>
     </row>
     <row r="2" spans="1:66" s="7" customFormat="1" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="303" t="s">
+      <c r="A2" s="323" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="305" t="s">
+      <c r="B2" s="325" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="305" t="s">
+      <c r="C2" s="325" t="s">
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -11873,9 +11961,9 @@
       <c r="BN2" s="6"/>
     </row>
     <row r="3" spans="1:66" s="7" customFormat="1" ht="101.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="304"/>
-      <c r="B3" s="306"/>
-      <c r="C3" s="306"/>
+      <c r="A3" s="324"/>
+      <c r="B3" s="326"/>
+      <c r="C3" s="326"/>
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
@@ -11949,9 +12037,9 @@
       <c r="BN3" s="6"/>
     </row>
     <row r="4" spans="1:66" s="7" customFormat="1" ht="152.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="304"/>
-      <c r="B4" s="306"/>
-      <c r="C4" s="306"/>
+      <c r="A4" s="324"/>
+      <c r="B4" s="326"/>
+      <c r="C4" s="326"/>
       <c r="D4" s="2" t="s">
         <v>18</v>
       </c>
@@ -12025,13 +12113,13 @@
       <c r="BN4" s="6"/>
     </row>
     <row r="5" spans="1:66" s="12" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="307" t="s">
+      <c r="A5" s="327" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="309" t="s">
+      <c r="B5" s="329" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="309" t="s">
+      <c r="C5" s="329" t="s">
         <v>24</v>
       </c>
       <c r="D5" s="8" t="s">
@@ -12107,9 +12195,9 @@
       <c r="BN5" s="6"/>
     </row>
     <row r="6" spans="1:66" s="12" customFormat="1" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="308"/>
-      <c r="B6" s="310"/>
-      <c r="C6" s="310"/>
+      <c r="A6" s="328"/>
+      <c r="B6" s="330"/>
+      <c r="C6" s="330"/>
       <c r="D6" s="15" t="s">
         <v>29</v>
       </c>
@@ -12183,9 +12271,9 @@
       <c r="BN6" s="6"/>
     </row>
     <row r="7" spans="1:66" s="12" customFormat="1" ht="171" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="308"/>
-      <c r="B7" s="310"/>
-      <c r="C7" s="310"/>
+      <c r="A7" s="328"/>
+      <c r="B7" s="330"/>
+      <c r="C7" s="330"/>
       <c r="D7" s="13" t="s">
         <v>33</v>
       </c>
@@ -12259,13 +12347,13 @@
       <c r="BN7" s="6"/>
     </row>
     <row r="8" spans="1:66" s="25" customFormat="1" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="318" t="s">
+      <c r="A8" s="312" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="320" t="s">
+      <c r="B8" s="314" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="320" t="s">
+      <c r="C8" s="314" t="s">
         <v>39</v>
       </c>
       <c r="D8" s="21" t="s">
@@ -12341,9 +12429,9 @@
       <c r="BN8" s="6"/>
     </row>
     <row r="9" spans="1:66" s="25" customFormat="1" ht="139.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="319"/>
-      <c r="B9" s="321"/>
-      <c r="C9" s="321"/>
+      <c r="A9" s="313"/>
+      <c r="B9" s="315"/>
+      <c r="C9" s="315"/>
       <c r="D9" s="21" t="s">
         <v>44</v>
       </c>
@@ -12417,9 +12505,9 @@
       <c r="BN9" s="6"/>
     </row>
     <row r="10" spans="1:66" s="25" customFormat="1" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="319"/>
-      <c r="B10" s="321"/>
-      <c r="C10" s="321"/>
+      <c r="A10" s="313"/>
+      <c r="B10" s="315"/>
+      <c r="C10" s="315"/>
       <c r="D10" s="21" t="s">
         <v>48</v>
       </c>
@@ -12493,9 +12581,9 @@
       <c r="BN10" s="6"/>
     </row>
     <row r="11" spans="1:66" s="25" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="319"/>
-      <c r="B11" s="321"/>
-      <c r="C11" s="322"/>
+      <c r="A11" s="313"/>
+      <c r="B11" s="315"/>
+      <c r="C11" s="316"/>
       <c r="D11" s="26" t="s">
         <v>52</v>
       </c>
@@ -12569,13 +12657,13 @@
       <c r="BN11" s="6"/>
     </row>
     <row r="12" spans="1:66" s="34" customFormat="1" ht="77.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="323" t="s">
+      <c r="A12" s="317" t="s">
         <v>56</v>
       </c>
-      <c r="B12" s="325" t="s">
+      <c r="B12" s="319" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="327" t="s">
+      <c r="C12" s="321" t="s">
         <v>58</v>
       </c>
       <c r="D12" s="30" t="s">
@@ -12651,9 +12739,9 @@
       <c r="BN12" s="6"/>
     </row>
     <row r="13" spans="1:66" s="34" customFormat="1" ht="85.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="324"/>
-      <c r="B13" s="326"/>
-      <c r="C13" s="328"/>
+      <c r="A13" s="318"/>
+      <c r="B13" s="320"/>
+      <c r="C13" s="322"/>
       <c r="D13" s="84" t="s">
         <v>63</v>
       </c>
@@ -12727,13 +12815,13 @@
       <c r="BN13" s="6"/>
     </row>
     <row r="14" spans="1:66" s="39" customFormat="1" ht="165" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="311" t="s">
+      <c r="A14" s="305" t="s">
         <v>67</v>
       </c>
-      <c r="B14" s="314" t="s">
+      <c r="B14" s="308" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="314" t="s">
+      <c r="C14" s="308" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="35" t="s">
@@ -12809,9 +12897,9 @@
       <c r="BN14" s="6"/>
     </row>
     <row r="15" spans="1:66" s="39" customFormat="1" ht="173.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="312"/>
-      <c r="B15" s="315"/>
-      <c r="C15" s="315"/>
+      <c r="A15" s="306"/>
+      <c r="B15" s="309"/>
+      <c r="C15" s="309"/>
       <c r="D15" s="40" t="s">
         <v>74</v>
       </c>
@@ -12885,9 +12973,9 @@
       <c r="BN15" s="6"/>
     </row>
     <row r="16" spans="1:66" s="39" customFormat="1" ht="214.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="313"/>
-      <c r="B16" s="316"/>
-      <c r="C16" s="317"/>
+      <c r="A16" s="307"/>
+      <c r="B16" s="310"/>
+      <c r="C16" s="311"/>
       <c r="D16" s="44" t="s">
         <v>78</v>
       </c>
@@ -13001,6 +13089,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="B14:B16"/>
     <mergeCell ref="C14:C16"/>
@@ -13010,12 +13104,6 @@
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -13058,10 +13146,10 @@
       <c r="M1" s="80"/>
     </row>
     <row r="2" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="334" t="s">
+      <c r="A2" s="336" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="329" t="s">
+      <c r="B2" s="331" t="s">
         <v>88</v>
       </c>
       <c r="C2" s="94" t="s">
@@ -13075,8 +13163,8 @@
       <c r="M2" s="81"/>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="332"/>
-      <c r="B3" s="331"/>
+      <c r="A3" s="334"/>
+      <c r="B3" s="332"/>
       <c r="C3" s="95"/>
       <c r="D3" s="103"/>
       <c r="E3" s="88" t="s">
@@ -13086,8 +13174,8 @@
       <c r="M3" s="81"/>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="332"/>
-      <c r="B4" s="331"/>
+      <c r="A4" s="334"/>
+      <c r="B4" s="332"/>
       <c r="C4" s="95" t="s">
         <v>92</v>
       </c>
@@ -13099,8 +13187,8 @@
       <c r="M4" s="80"/>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="332"/>
-      <c r="B5" s="331"/>
+      <c r="A5" s="334"/>
+      <c r="B5" s="332"/>
       <c r="C5" s="95"/>
       <c r="D5" s="103"/>
       <c r="E5" s="88" t="s">
@@ -13110,8 +13198,8 @@
       <c r="M5" s="81"/>
     </row>
     <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="332"/>
-      <c r="B6" s="331"/>
+      <c r="A6" s="334"/>
+      <c r="B6" s="332"/>
       <c r="C6" s="95"/>
       <c r="D6" s="103"/>
       <c r="E6" s="88" t="s">
@@ -13121,8 +13209,8 @@
       <c r="M6" s="81"/>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="332"/>
-      <c r="B7" s="331"/>
+      <c r="A7" s="334"/>
+      <c r="B7" s="332"/>
       <c r="C7" s="95"/>
       <c r="D7" s="103"/>
       <c r="E7" s="88" t="s">
@@ -13132,8 +13220,8 @@
       <c r="M7" s="81"/>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="332"/>
-      <c r="B8" s="331"/>
+      <c r="A8" s="334"/>
+      <c r="B8" s="332"/>
       <c r="C8" s="95" t="s">
         <v>97</v>
       </c>
@@ -13145,8 +13233,8 @@
       <c r="M8" s="81"/>
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="332"/>
-      <c r="B9" s="331"/>
+      <c r="A9" s="334"/>
+      <c r="B9" s="332"/>
       <c r="C9" s="95"/>
       <c r="D9" s="103"/>
       <c r="E9" s="88" t="s">
@@ -13156,8 +13244,8 @@
       <c r="M9" s="81"/>
     </row>
     <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="332"/>
-      <c r="B10" s="331"/>
+      <c r="A10" s="334"/>
+      <c r="B10" s="332"/>
       <c r="C10" s="95"/>
       <c r="D10" s="103"/>
       <c r="E10" s="88" t="s">
@@ -13167,8 +13255,8 @@
       <c r="M10" s="81"/>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="332"/>
-      <c r="B11" s="331"/>
+      <c r="A11" s="334"/>
+      <c r="B11" s="332"/>
       <c r="C11" s="95" t="s">
         <v>101</v>
       </c>
@@ -13180,8 +13268,8 @@
       <c r="M11" s="81"/>
     </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="332"/>
-      <c r="B12" s="331"/>
+      <c r="A12" s="334"/>
+      <c r="B12" s="332"/>
       <c r="C12" s="95"/>
       <c r="D12" s="103"/>
       <c r="E12" s="88" t="s">
@@ -13191,8 +13279,8 @@
       <c r="M12" s="81"/>
     </row>
     <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="333"/>
-      <c r="B13" s="330"/>
+      <c r="A13" s="335"/>
+      <c r="B13" s="333"/>
       <c r="C13" s="96"/>
       <c r="D13" s="104"/>
       <c r="E13" s="89" t="s">
@@ -13202,10 +13290,10 @@
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="332" t="s">
+      <c r="A14" s="334" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="329" t="s">
+      <c r="B14" s="331" t="s">
         <v>106</v>
       </c>
       <c r="C14" s="95" t="s">
@@ -13219,8 +13307,8 @@
       <c r="M14" s="81"/>
     </row>
     <row r="15" spans="1:13" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="333"/>
-      <c r="B15" s="330"/>
+      <c r="A15" s="335"/>
+      <c r="B15" s="333"/>
       <c r="C15" s="96"/>
       <c r="D15" s="104"/>
       <c r="E15" s="89" t="s">
@@ -13230,10 +13318,10 @@
       <c r="M15" s="81"/>
     </row>
     <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="332" t="s">
+      <c r="A16" s="334" t="s">
         <v>110</v>
       </c>
-      <c r="B16" s="329" t="s">
+      <c r="B16" s="331" t="s">
         <v>111</v>
       </c>
       <c r="C16" s="95" t="s">
@@ -13247,8 +13335,8 @@
       <c r="M16" s="81"/>
     </row>
     <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="332"/>
-      <c r="B17" s="331"/>
+      <c r="A17" s="334"/>
+      <c r="B17" s="332"/>
       <c r="C17" s="95"/>
       <c r="D17" s="103"/>
       <c r="E17" s="88" t="s">
@@ -13258,8 +13346,8 @@
       <c r="M17" s="81"/>
     </row>
     <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="332"/>
-      <c r="B18" s="331"/>
+      <c r="A18" s="334"/>
+      <c r="B18" s="332"/>
       <c r="C18" s="95"/>
       <c r="D18" s="103"/>
       <c r="E18" s="88" t="s">
@@ -13269,8 +13357,8 @@
       <c r="M18" s="81"/>
     </row>
     <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="332"/>
-      <c r="B19" s="331"/>
+      <c r="A19" s="334"/>
+      <c r="B19" s="332"/>
       <c r="C19" s="95" t="s">
         <v>115</v>
       </c>
@@ -13282,8 +13370,8 @@
       <c r="M19" s="81"/>
     </row>
     <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="332"/>
-      <c r="B20" s="331"/>
+      <c r="A20" s="334"/>
+      <c r="B20" s="332"/>
       <c r="C20" s="95"/>
       <c r="D20" s="103"/>
       <c r="E20" s="88" t="s">
@@ -13293,8 +13381,8 @@
       <c r="M20" s="81"/>
     </row>
     <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="332"/>
-      <c r="B21" s="331"/>
+      <c r="A21" s="334"/>
+      <c r="B21" s="332"/>
       <c r="C21" s="95"/>
       <c r="D21" s="103"/>
       <c r="E21" s="88" t="s">
@@ -13304,8 +13392,8 @@
       <c r="M21" s="81"/>
     </row>
     <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="332"/>
-      <c r="B22" s="331"/>
+      <c r="A22" s="334"/>
+      <c r="B22" s="332"/>
       <c r="C22" s="95" t="s">
         <v>119</v>
       </c>
@@ -13317,8 +13405,8 @@
       <c r="M22" s="80"/>
     </row>
     <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="332"/>
-      <c r="B23" s="330"/>
+      <c r="A23" s="334"/>
+      <c r="B23" s="333"/>
       <c r="C23" s="95"/>
       <c r="D23" s="103"/>
       <c r="E23" s="88" t="s">
@@ -13345,10 +13433,10 @@
       <c r="M24" s="81"/>
     </row>
     <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="332" t="s">
+      <c r="A25" s="334" t="s">
         <v>126</v>
       </c>
-      <c r="B25" s="329" t="s">
+      <c r="B25" s="331" t="s">
         <v>127</v>
       </c>
       <c r="C25" s="95" t="s">
@@ -13362,8 +13450,8 @@
       <c r="M25" s="81"/>
     </row>
     <row r="26" spans="1:13" ht="97.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="333"/>
-      <c r="B26" s="330"/>
+      <c r="A26" s="335"/>
+      <c r="B26" s="333"/>
       <c r="C26" s="96"/>
       <c r="D26" s="104"/>
       <c r="E26" s="89" t="s">
@@ -13373,10 +13461,10 @@
       <c r="M26" s="81"/>
     </row>
     <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="332" t="s">
+      <c r="A27" s="334" t="s">
         <v>131</v>
       </c>
-      <c r="B27" s="329" t="s">
+      <c r="B27" s="331" t="s">
         <v>132</v>
       </c>
       <c r="C27" s="95" t="s">
@@ -13390,8 +13478,8 @@
       <c r="M27" s="81"/>
     </row>
     <row r="28" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A28" s="332"/>
-      <c r="B28" s="331"/>
+      <c r="A28" s="334"/>
+      <c r="B28" s="332"/>
       <c r="C28" s="95"/>
       <c r="D28" s="103"/>
       <c r="E28" s="88" t="s">
@@ -13401,8 +13489,8 @@
       <c r="M28" s="81"/>
     </row>
     <row r="29" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A29" s="333"/>
-      <c r="B29" s="330"/>
+      <c r="A29" s="335"/>
+      <c r="B29" s="333"/>
       <c r="C29" s="96"/>
       <c r="D29" s="104"/>
       <c r="E29" s="89" t="s">
@@ -13411,10 +13499,10 @@
       <c r="M29" s="81"/>
     </row>
     <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="332" t="s">
+      <c r="A30" s="334" t="s">
         <v>137</v>
       </c>
-      <c r="B30" s="329" t="s">
+      <c r="B30" s="331" t="s">
         <v>138</v>
       </c>
       <c r="C30" s="95" t="s">
@@ -13427,8 +13515,8 @@
       <c r="M30" s="81"/>
     </row>
     <row r="31" spans="1:13" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="333"/>
-      <c r="B31" s="330"/>
+      <c r="A31" s="335"/>
+      <c r="B31" s="333"/>
       <c r="C31" s="96"/>
       <c r="D31" s="104"/>
       <c r="E31" s="89" t="s">
@@ -13437,10 +13525,10 @@
       <c r="M31" s="81"/>
     </row>
     <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="332" t="s">
+      <c r="A32" s="334" t="s">
         <v>141</v>
       </c>
-      <c r="B32" s="329" t="s">
+      <c r="B32" s="331" t="s">
         <v>142</v>
       </c>
       <c r="C32" s="95" t="s">
@@ -13453,8 +13541,8 @@
       <c r="M32" s="81"/>
     </row>
     <row r="33" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A33" s="332"/>
-      <c r="B33" s="331"/>
+      <c r="A33" s="334"/>
+      <c r="B33" s="332"/>
       <c r="C33" s="95" t="s">
         <v>144</v>
       </c>
@@ -13465,8 +13553,8 @@
       <c r="M33" s="81"/>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="332"/>
-      <c r="B34" s="331"/>
+      <c r="A34" s="334"/>
+      <c r="B34" s="332"/>
       <c r="C34" s="95"/>
       <c r="D34" s="103"/>
       <c r="E34" s="88" t="s">
@@ -13475,8 +13563,8 @@
       <c r="M34" s="81"/>
     </row>
     <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="332"/>
-      <c r="B35" s="331"/>
+      <c r="A35" s="334"/>
+      <c r="B35" s="332"/>
       <c r="C35" s="95"/>
       <c r="D35" s="103"/>
       <c r="E35" s="88" t="s">
@@ -13485,8 +13573,8 @@
       <c r="M35" s="81"/>
     </row>
     <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="333"/>
-      <c r="B36" s="330"/>
+      <c r="A36" s="335"/>
+      <c r="B36" s="333"/>
       <c r="C36" s="96"/>
       <c r="D36" s="104"/>
       <c r="E36" s="89" t="s">
@@ -13495,10 +13583,10 @@
       <c r="M36" s="81"/>
     </row>
     <row r="37" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="335" t="s">
+      <c r="A37" s="337" t="s">
         <v>149</v>
       </c>
-      <c r="B37" s="329" t="s">
+      <c r="B37" s="331" t="s">
         <v>150</v>
       </c>
       <c r="C37" s="95" t="s">
@@ -13511,8 +13599,8 @@
       <c r="M37" s="81"/>
     </row>
     <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="335"/>
-      <c r="B38" s="331"/>
+      <c r="A38" s="337"/>
+      <c r="B38" s="332"/>
       <c r="C38" s="95"/>
       <c r="D38" s="103"/>
       <c r="E38" s="88" t="s">
@@ -13521,8 +13609,8 @@
       <c r="M38" s="81"/>
     </row>
     <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="335"/>
-      <c r="B39" s="331"/>
+      <c r="A39" s="337"/>
+      <c r="B39" s="332"/>
       <c r="C39" s="95"/>
       <c r="D39" s="103"/>
       <c r="E39" s="88" t="s">
@@ -13531,8 +13619,8 @@
       <c r="M39" s="81"/>
     </row>
     <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="335"/>
-      <c r="B40" s="331"/>
+      <c r="A40" s="337"/>
+      <c r="B40" s="332"/>
       <c r="C40" s="95" t="s">
         <v>107</v>
       </c>
@@ -13543,8 +13631,8 @@
       <c r="M40" s="81"/>
     </row>
     <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="335"/>
-      <c r="B41" s="331"/>
+      <c r="A41" s="337"/>
+      <c r="B41" s="332"/>
       <c r="C41" s="95"/>
       <c r="D41" s="103"/>
       <c r="E41" s="88" t="s">
@@ -13553,8 +13641,8 @@
       <c r="M41" s="81"/>
     </row>
     <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="335"/>
-      <c r="B42" s="331"/>
+      <c r="A42" s="337"/>
+      <c r="B42" s="332"/>
       <c r="C42" s="95"/>
       <c r="D42" s="103"/>
       <c r="E42" s="88" t="s">
@@ -13563,8 +13651,8 @@
       <c r="M42" s="81"/>
     </row>
     <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="335"/>
-      <c r="B43" s="331"/>
+      <c r="A43" s="337"/>
+      <c r="B43" s="332"/>
       <c r="C43" s="95" t="s">
         <v>154</v>
       </c>
@@ -13575,8 +13663,8 @@
       <c r="M43" s="81"/>
     </row>
     <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="335"/>
-      <c r="B44" s="331"/>
+      <c r="A44" s="337"/>
+      <c r="B44" s="332"/>
       <c r="C44" s="95"/>
       <c r="D44" s="103"/>
       <c r="E44" s="88" t="s">
@@ -13585,8 +13673,8 @@
       <c r="M44" s="81"/>
     </row>
     <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A45" s="335"/>
-      <c r="B45" s="331"/>
+      <c r="A45" s="337"/>
+      <c r="B45" s="332"/>
       <c r="C45" s="95"/>
       <c r="D45" s="103"/>
       <c r="E45" s="88" t="s">
@@ -13595,8 +13683,8 @@
       <c r="M45" s="81"/>
     </row>
     <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="336"/>
-      <c r="B46" s="330"/>
+      <c r="A46" s="338"/>
+      <c r="B46" s="333"/>
       <c r="C46" s="96"/>
       <c r="D46" s="104"/>
       <c r="E46" s="91" t="s">
@@ -13605,10 +13693,10 @@
       <c r="M46" s="81"/>
     </row>
     <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="332" t="s">
+      <c r="A47" s="334" t="s">
         <v>157</v>
       </c>
-      <c r="B47" s="329" t="s">
+      <c r="B47" s="331" t="s">
         <v>158</v>
       </c>
       <c r="C47" s="95" t="s">
@@ -13621,8 +13709,8 @@
       <c r="M47" s="81"/>
     </row>
     <row r="48" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="332"/>
-      <c r="B48" s="331"/>
+      <c r="A48" s="334"/>
+      <c r="B48" s="332"/>
       <c r="C48" s="95"/>
       <c r="D48" s="103"/>
       <c r="E48" s="92" t="s">
@@ -13631,8 +13719,8 @@
       <c r="M48" s="81"/>
     </row>
     <row r="49" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="332"/>
-      <c r="B49" s="331"/>
+      <c r="A49" s="334"/>
+      <c r="B49" s="332"/>
       <c r="C49" s="95" t="s">
         <v>107</v>
       </c>
@@ -13643,8 +13731,8 @@
       <c r="M49" s="81"/>
     </row>
     <row r="50" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="332"/>
-      <c r="B50" s="331"/>
+      <c r="A50" s="334"/>
+      <c r="B50" s="332"/>
       <c r="C50" s="95" t="s">
         <v>115</v>
       </c>
@@ -13655,8 +13743,8 @@
       <c r="M50" s="80"/>
     </row>
     <row r="51" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="332"/>
-      <c r="B51" s="331"/>
+      <c r="A51" s="334"/>
+      <c r="B51" s="332"/>
       <c r="C51" s="95"/>
       <c r="D51" s="103"/>
       <c r="E51" s="92" t="s">
@@ -13665,8 +13753,8 @@
       <c r="M51" s="81"/>
     </row>
     <row r="52" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="332"/>
-      <c r="B52" s="331"/>
+      <c r="A52" s="334"/>
+      <c r="B52" s="332"/>
       <c r="C52" s="95"/>
       <c r="D52" s="103"/>
       <c r="E52" s="92" t="s">
@@ -13675,8 +13763,8 @@
       <c r="M52" s="80"/>
     </row>
     <row r="53" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="332"/>
-      <c r="B53" s="331"/>
+      <c r="A53" s="334"/>
+      <c r="B53" s="332"/>
       <c r="C53" s="95"/>
       <c r="D53" s="103"/>
       <c r="E53" s="88" t="s">
@@ -13685,8 +13773,8 @@
       <c r="M53" s="81"/>
     </row>
     <row r="54" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A54" s="332"/>
-      <c r="B54" s="331"/>
+      <c r="A54" s="334"/>
+      <c r="B54" s="332"/>
       <c r="C54" s="95" t="s">
         <v>119</v>
       </c>
@@ -13697,8 +13785,8 @@
       <c r="M54" s="81"/>
     </row>
     <row r="55" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="332"/>
-      <c r="B55" s="331"/>
+      <c r="A55" s="334"/>
+      <c r="B55" s="332"/>
       <c r="C55" s="95" t="s">
         <v>167</v>
       </c>
@@ -13709,8 +13797,8 @@
       <c r="M55" s="81"/>
     </row>
     <row r="56" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="332"/>
-      <c r="B56" s="331"/>
+      <c r="A56" s="334"/>
+      <c r="B56" s="332"/>
       <c r="C56" s="95" t="s">
         <v>169</v>
       </c>
@@ -13721,8 +13809,8 @@
       <c r="M56" s="81"/>
     </row>
     <row r="57" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="332"/>
-      <c r="B57" s="331"/>
+      <c r="A57" s="334"/>
+      <c r="B57" s="332"/>
       <c r="C57" s="95" t="s">
         <v>170</v>
       </c>
@@ -13733,8 +13821,8 @@
       <c r="M57" s="80"/>
     </row>
     <row r="58" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A58" s="333"/>
-      <c r="B58" s="330"/>
+      <c r="A58" s="335"/>
+      <c r="B58" s="333"/>
       <c r="C58" s="96" t="s">
         <v>154</v>
       </c>
@@ -13745,10 +13833,10 @@
       <c r="M58" s="81"/>
     </row>
     <row r="59" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="332" t="s">
+      <c r="A59" s="334" t="s">
         <v>172</v>
       </c>
-      <c r="B59" s="329" t="s">
+      <c r="B59" s="331" t="s">
         <v>173</v>
       </c>
       <c r="C59" s="95" t="s">
@@ -13761,8 +13849,8 @@
       <c r="M59" s="81"/>
     </row>
     <row r="60" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="332"/>
-      <c r="B60" s="331"/>
+      <c r="A60" s="334"/>
+      <c r="B60" s="332"/>
       <c r="C60" s="95"/>
       <c r="D60" s="103"/>
       <c r="E60" s="88" t="s">
@@ -13771,8 +13859,8 @@
       <c r="M60" s="81"/>
     </row>
     <row r="61" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="332"/>
-      <c r="B61" s="331"/>
+      <c r="A61" s="334"/>
+      <c r="B61" s="332"/>
       <c r="C61" s="95" t="s">
         <v>154</v>
       </c>
@@ -13783,8 +13871,8 @@
       <c r="M61" s="81"/>
     </row>
     <row r="62" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="333"/>
-      <c r="B62" s="330"/>
+      <c r="A62" s="335"/>
+      <c r="B62" s="333"/>
       <c r="C62" s="96"/>
       <c r="D62" s="104"/>
       <c r="E62" s="89" t="s">
@@ -13793,10 +13881,10 @@
       <c r="M62" s="80"/>
     </row>
     <row r="63" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="332" t="s">
+      <c r="A63" s="334" t="s">
         <v>175</v>
       </c>
-      <c r="B63" s="329" t="s">
+      <c r="B63" s="331" t="s">
         <v>176</v>
       </c>
       <c r="C63" s="95" t="s">
@@ -13809,8 +13897,8 @@
       <c r="M63" s="81"/>
     </row>
     <row r="64" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="332"/>
-      <c r="B64" s="331"/>
+      <c r="A64" s="334"/>
+      <c r="B64" s="332"/>
       <c r="C64" s="95"/>
       <c r="D64" s="103"/>
       <c r="E64" s="88" t="s">
@@ -13820,8 +13908,8 @@
       <c r="M64" s="81"/>
     </row>
     <row r="65" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="332"/>
-      <c r="B65" s="331"/>
+      <c r="A65" s="334"/>
+      <c r="B65" s="332"/>
       <c r="C65" s="95"/>
       <c r="D65" s="103"/>
       <c r="E65" s="88" t="s">
@@ -13831,8 +13919,8 @@
       <c r="M65" s="81"/>
     </row>
     <row r="66" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A66" s="332"/>
-      <c r="B66" s="331"/>
+      <c r="A66" s="334"/>
+      <c r="B66" s="332"/>
       <c r="C66" s="95" t="s">
         <v>107</v>
       </c>
@@ -13844,8 +13932,8 @@
       <c r="M66" s="81"/>
     </row>
     <row r="67" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="332"/>
-      <c r="B67" s="331"/>
+      <c r="A67" s="334"/>
+      <c r="B67" s="332"/>
       <c r="C67" s="95" t="s">
         <v>119</v>
       </c>
@@ -13857,8 +13945,8 @@
       <c r="M67" s="81"/>
     </row>
     <row r="68" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="332"/>
-      <c r="B68" s="331"/>
+      <c r="A68" s="334"/>
+      <c r="B68" s="332"/>
       <c r="C68" s="95" t="s">
         <v>170</v>
       </c>
@@ -13870,8 +13958,8 @@
       <c r="M68" s="81"/>
     </row>
     <row r="69" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="332"/>
-      <c r="B69" s="331"/>
+      <c r="A69" s="334"/>
+      <c r="B69" s="332"/>
       <c r="C69" s="95" t="s">
         <v>154</v>
       </c>
@@ -13883,8 +13971,8 @@
       <c r="M69" s="81"/>
     </row>
     <row r="70" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="332"/>
-      <c r="B70" s="331"/>
+      <c r="A70" s="334"/>
+      <c r="B70" s="332"/>
       <c r="C70" s="95"/>
       <c r="D70" s="103"/>
       <c r="E70" s="88" t="s">
@@ -13894,8 +13982,8 @@
       <c r="M70" s="80"/>
     </row>
     <row r="71" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A71" s="333"/>
-      <c r="B71" s="330"/>
+      <c r="A71" s="335"/>
+      <c r="B71" s="333"/>
       <c r="C71" s="96" t="s">
         <v>101</v>
       </c>
@@ -13907,10 +13995,10 @@
       <c r="M71" s="81"/>
     </row>
     <row r="72" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="332" t="s">
+      <c r="A72" s="334" t="s">
         <v>186</v>
       </c>
-      <c r="B72" s="329" t="s">
+      <c r="B72" s="331" t="s">
         <v>187</v>
       </c>
       <c r="C72" s="95" t="s">
@@ -13924,8 +14012,8 @@
       <c r="M72" s="81"/>
     </row>
     <row r="73" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="332"/>
-      <c r="B73" s="331"/>
+      <c r="A73" s="334"/>
+      <c r="B73" s="332"/>
       <c r="C73" s="95"/>
       <c r="D73" s="103"/>
       <c r="E73" s="92" t="s">
@@ -13935,8 +14023,8 @@
       <c r="M73" s="81"/>
     </row>
     <row r="74" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="332"/>
-      <c r="B74" s="331"/>
+      <c r="A74" s="334"/>
+      <c r="B74" s="332"/>
       <c r="C74" s="95" t="s">
         <v>190</v>
       </c>
@@ -13948,8 +14036,8 @@
       <c r="M74" s="81"/>
     </row>
     <row r="75" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="332"/>
-      <c r="B75" s="331"/>
+      <c r="A75" s="334"/>
+      <c r="B75" s="332"/>
       <c r="C75" s="95"/>
       <c r="D75" s="103"/>
       <c r="E75" s="92" t="s">
@@ -13959,8 +14047,8 @@
       <c r="M75" s="81"/>
     </row>
     <row r="76" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="332"/>
-      <c r="B76" s="331"/>
+      <c r="A76" s="334"/>
+      <c r="B76" s="332"/>
       <c r="C76" s="95"/>
       <c r="D76" s="103"/>
       <c r="E76" s="92" t="s">
@@ -13970,8 +14058,8 @@
       <c r="M76" s="80"/>
     </row>
     <row r="77" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="332"/>
-      <c r="B77" s="331"/>
+      <c r="A77" s="334"/>
+      <c r="B77" s="332"/>
       <c r="C77" s="95" t="s">
         <v>167</v>
       </c>
@@ -13983,8 +14071,8 @@
       <c r="M77" s="81"/>
     </row>
     <row r="78" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="332"/>
-      <c r="B78" s="331"/>
+      <c r="A78" s="334"/>
+      <c r="B78" s="332"/>
       <c r="C78" s="95"/>
       <c r="D78" s="103"/>
       <c r="E78" s="92" t="s">
@@ -13994,8 +14082,8 @@
       <c r="M78" s="81"/>
     </row>
     <row r="79" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A79" s="332"/>
-      <c r="B79" s="331"/>
+      <c r="A79" s="334"/>
+      <c r="B79" s="332"/>
       <c r="C79" s="95"/>
       <c r="D79" s="103"/>
       <c r="E79" s="92" t="s">
@@ -14005,8 +14093,8 @@
       <c r="M79" s="80"/>
     </row>
     <row r="80" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A80" s="332"/>
-      <c r="B80" s="331"/>
+      <c r="A80" s="334"/>
+      <c r="B80" s="332"/>
       <c r="C80" s="95" t="s">
         <v>169</v>
       </c>
@@ -14018,8 +14106,8 @@
       <c r="M80" s="81"/>
     </row>
     <row r="81" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="332"/>
-      <c r="B81" s="331"/>
+      <c r="A81" s="334"/>
+      <c r="B81" s="332"/>
       <c r="C81" s="95"/>
       <c r="D81" s="103"/>
       <c r="E81" s="92" t="s">
@@ -14029,8 +14117,8 @@
       <c r="M81" s="81"/>
     </row>
     <row r="82" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="333"/>
-      <c r="B82" s="330"/>
+      <c r="A82" s="335"/>
+      <c r="B82" s="333"/>
       <c r="C82" s="96"/>
       <c r="D82" s="104"/>
       <c r="E82" s="91" t="s">
@@ -14223,12 +14311,12 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B72:B82"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B37:B46"/>
-    <mergeCell ref="B47:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B71"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B29"/>
     <mergeCell ref="A72:A82"/>
     <mergeCell ref="A2:A13"/>
     <mergeCell ref="A14:A15"/>
@@ -14241,12 +14329,12 @@
     <mergeCell ref="A47:A58"/>
     <mergeCell ref="A59:A62"/>
     <mergeCell ref="A63:A71"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B2:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B72:B82"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B37:B46"/>
+    <mergeCell ref="B47:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -23568,9 +23656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B771BD26-5CB2-F242-A0FA-A4D8589272A0}">
   <dimension ref="A1:BO73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H66" sqref="H66"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M65" sqref="M65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -23585,6 +23673,8 @@
     <col min="9" max="9" width="31.6640625" style="128" customWidth="1"/>
     <col min="10" max="10" width="97" customWidth="1"/>
     <col min="11" max="11" width="36.1640625" customWidth="1"/>
+    <col min="12" max="12" width="25" style="185" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" style="185" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" s="1" customFormat="1" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -23618,11 +23708,15 @@
       <c r="J1" s="114" t="s">
         <v>385</v>
       </c>
-      <c r="K1" s="338" t="s">
+      <c r="K1" s="304" t="s">
         <v>390</v>
       </c>
-      <c r="L1" s="114"/>
-      <c r="M1" s="114"/>
+      <c r="L1" s="340" t="s">
+        <v>483</v>
+      </c>
+      <c r="M1" s="341" t="s">
+        <v>484</v>
+      </c>
       <c r="N1" s="114"/>
       <c r="O1" s="114"/>
       <c r="P1" s="114"/>
@@ -23707,15 +23801,21 @@
         <v>87</v>
       </c>
       <c r="J2" s="126" t="str">
-        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K2" s="126" t="str">
-        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L2" s="114"/>
-      <c r="M2" s="114"/>
+        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L2" s="342" t="str">
+        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M2" s="343" t="str">
+        <f>VLOOKUP(I2,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N2" s="114"/>
       <c r="O2" s="114"/>
       <c r="P2" s="114"/>
@@ -23800,15 +23900,21 @@
         <v>87</v>
       </c>
       <c r="J3" s="126" t="str">
-        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K3" s="126" t="str">
-        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
+        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L3" s="342" t="str">
+        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M3" s="343" t="str">
+        <f>VLOOKUP(I3,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N3" s="114"/>
       <c r="O3" s="114"/>
       <c r="P3" s="114"/>
@@ -23893,15 +23999,21 @@
         <v>175</v>
       </c>
       <c r="J4" s="126" t="str">
-        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K4" s="126" t="str">
-        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L4" s="114"/>
-      <c r="M4" s="114"/>
+      <c r="L4" s="342" t="str">
+        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M4" s="343" t="str">
+        <f>VLOOKUP(I4,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N4" s="114"/>
       <c r="O4" s="114"/>
       <c r="P4" s="114"/>
@@ -23986,15 +24098,21 @@
         <v>175</v>
       </c>
       <c r="J5" s="126" t="str">
-        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K5" s="126" t="str">
-        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L5" s="117"/>
-      <c r="M5" s="117"/>
+      <c r="L5" s="342" t="str">
+        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M5" s="343" t="str">
+        <f>VLOOKUP(I5,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N5" s="117"/>
       <c r="O5" s="117"/>
       <c r="P5" s="117"/>
@@ -24079,15 +24197,21 @@
         <v>319</v>
       </c>
       <c r="J6" s="126" t="e">
-        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="K6" s="126" t="e">
-        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>#N/A</v>
       </c>
-      <c r="L6" s="117"/>
-      <c r="M6" s="117"/>
+      <c r="L6" s="342" t="e">
+        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M6" s="343" t="e">
+        <f>VLOOKUP(I6,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>#N/A</v>
+      </c>
       <c r="N6" s="117"/>
       <c r="O6" s="117"/>
       <c r="P6" s="117"/>
@@ -24172,15 +24296,21 @@
         <v>126</v>
       </c>
       <c r="J7" s="126" t="str">
-        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Campaign Manager allows the segmentation of participants according to different characteristics e.g. demographics or clinical risk factors and tailor screening pathway outreach accordingly to maximise uptake. It enables personalisation of health communication campaigns and allows the impact of these campaigns to be assessed.</v>
       </c>
       <c r="K7" s="126" t="str">
-        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L7" s="117"/>
-      <c r="M7" s="117"/>
+      <c r="L7" s="342" t="str">
+        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Marketing</v>
+      </c>
+      <c r="M7" s="343" t="str">
+        <f>VLOOKUP(I7,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Campaign</v>
+      </c>
       <c r="N7" s="117"/>
       <c r="O7" s="117"/>
       <c r="P7" s="117"/>
@@ -24265,15 +24395,21 @@
         <v>126</v>
       </c>
       <c r="J8" s="126" t="str">
-        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Campaign Manager allows the segmentation of participants according to different characteristics e.g. demographics or clinical risk factors and tailor screening pathway outreach accordingly to maximise uptake. It enables personalisation of health communication campaigns and allows the impact of these campaigns to be assessed.</v>
       </c>
       <c r="K8" s="126" t="str">
-        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L8" s="117"/>
-      <c r="M8" s="117"/>
+      <c r="L8" s="342" t="str">
+        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Marketing</v>
+      </c>
+      <c r="M8" s="343" t="str">
+        <f>VLOOKUP(I8,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Campaign</v>
+      </c>
       <c r="N8" s="117"/>
       <c r="O8" s="117"/>
       <c r="P8" s="117"/>
@@ -24358,15 +24494,21 @@
         <v>87</v>
       </c>
       <c r="J9" s="126" t="str">
-        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K9" s="126" t="str">
-        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L9" s="117"/>
-      <c r="M9" s="117"/>
+        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L9" s="342" t="str">
+        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M9" s="343" t="str">
+        <f>VLOOKUP(I9,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N9" s="117"/>
       <c r="O9" s="117"/>
       <c r="P9" s="117"/>
@@ -24451,15 +24593,21 @@
         <v>137</v>
       </c>
       <c r="J10" s="126" t="str">
-        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity Manager provides a centralised way of understanding and managing capacity across screening pathways. Providers are able to provide and amend their local capacity, with resulting available 'slots' feeding into the allocation process.</v>
       </c>
       <c r="K10" s="126" t="str">
-        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L10" s="117"/>
-      <c r="M10" s="117"/>
+      <c r="L10" s="342" t="str">
+        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity</v>
+      </c>
+      <c r="M10" s="343" t="str">
+        <f>VLOOKUP(I10,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Slot</v>
+      </c>
       <c r="N10" s="117"/>
       <c r="O10" s="117"/>
       <c r="P10" s="117"/>
@@ -24544,15 +24692,21 @@
         <v>141</v>
       </c>
       <c r="J11" s="126" t="str">
-        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
       <c r="K11" s="126" t="str">
-        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L11" s="117"/>
-      <c r="M11" s="117"/>
+      <c r="L11" s="342" t="str">
+        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M11" s="343" t="str">
+        <f>VLOOKUP(I11,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Invitable Participant</v>
+      </c>
       <c r="N11" s="117"/>
       <c r="O11" s="117"/>
       <c r="P11" s="117"/>
@@ -24637,15 +24791,21 @@
         <v>131</v>
       </c>
       <c r="J12" s="126" t="str">
-        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
       <c r="K12" s="126" t="str">
-        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L12" s="117"/>
-      <c r="M12" s="117"/>
+      <c r="L12" s="342" t="str">
+        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity/Demand</v>
+      </c>
+      <c r="M12" s="343" t="str">
+        <f>VLOOKUP(I12,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Provisional slot, Provisional appointment request</v>
+      </c>
       <c r="N12" s="117"/>
       <c r="O12" s="117"/>
       <c r="P12" s="117"/>
@@ -24730,15 +24890,21 @@
         <v>137</v>
       </c>
       <c r="J13" s="126" t="str">
-        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity Manager provides a centralised way of understanding and managing capacity across screening pathways. Providers are able to provide and amend their local capacity, with resulting available 'slots' feeding into the allocation process.</v>
       </c>
       <c r="K13" s="126" t="str">
-        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L13" s="117"/>
-      <c r="M13" s="117"/>
+      <c r="L13" s="342" t="str">
+        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity</v>
+      </c>
+      <c r="M13" s="343" t="str">
+        <f>VLOOKUP(I13,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Slot</v>
+      </c>
       <c r="N13" s="117"/>
       <c r="O13" s="117"/>
       <c r="P13" s="117"/>
@@ -24823,15 +24989,21 @@
         <v>131</v>
       </c>
       <c r="J14" s="126" t="str">
-        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
       <c r="K14" s="126" t="str">
-        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L14" s="117"/>
-      <c r="M14" s="117"/>
+      <c r="L14" s="342" t="str">
+        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity/Demand</v>
+      </c>
+      <c r="M14" s="343" t="str">
+        <f>VLOOKUP(I14,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Provisional slot, Provisional appointment request</v>
+      </c>
       <c r="N14" s="117"/>
       <c r="O14" s="117"/>
       <c r="P14" s="117"/>
@@ -24916,15 +25088,21 @@
         <v>131</v>
       </c>
       <c r="J15" s="126" t="str">
-        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
       <c r="K15" s="126" t="str">
-        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L15" s="117"/>
-      <c r="M15" s="117"/>
+      <c r="L15" s="342" t="str">
+        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity/Demand</v>
+      </c>
+      <c r="M15" s="343" t="str">
+        <f>VLOOKUP(I15,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Provisional slot, Provisional appointment request</v>
+      </c>
       <c r="N15" s="117"/>
       <c r="O15" s="117"/>
       <c r="P15" s="117"/>
@@ -25009,15 +25187,21 @@
         <v>131</v>
       </c>
       <c r="J16" s="126" t="str">
-        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Capacity and Demand Planner can model different demand and capacity scenarios to inform decision making. This provides visibility on potential mismatches e.g. a surge of demand due to a new campaign and provides critical information to provision capacity accordingly.</v>
       </c>
       <c r="K16" s="126" t="str">
-        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L16" s="117"/>
-      <c r="M16" s="117"/>
+      <c r="L16" s="342" t="str">
+        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Capacity/Demand</v>
+      </c>
+      <c r="M16" s="343" t="str">
+        <f>VLOOKUP(I16,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Provisional slot, Provisional appointment request</v>
+      </c>
       <c r="N16" s="117"/>
       <c r="O16" s="117"/>
       <c r="P16" s="117"/>
@@ -25101,16 +25285,22 @@
       <c r="I17" s="133" t="s">
         <v>320</v>
       </c>
-      <c r="J17" s="126" t="e">
-        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K17" s="126" t="e">
-        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L17" s="117"/>
-      <c r="M17" s="117"/>
+      <c r="J17" s="126" t="str">
+        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
+        <v>Cohorting as a Service manages cohort definitions and informs Cohort Manager when a participant changes in their eligibility status</v>
+      </c>
+      <c r="K17" s="126" t="str">
+        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Staff users</v>
+      </c>
+      <c r="L17" s="342" t="str">
+        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M17" s="343" t="str">
+        <f>VLOOKUP(I17,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Eligible Participant</v>
+      </c>
       <c r="N17" s="117"/>
       <c r="O17" s="117"/>
       <c r="P17" s="117"/>
@@ -25195,15 +25385,21 @@
         <v>175</v>
       </c>
       <c r="J18" s="126" t="str">
-        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K18" s="126" t="str">
-        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L18" s="117"/>
-      <c r="M18" s="117"/>
+      <c r="L18" s="342" t="str">
+        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M18" s="343" t="str">
+        <f>VLOOKUP(I18,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N18" s="117"/>
       <c r="O18" s="117"/>
       <c r="P18" s="117"/>
@@ -25288,15 +25484,21 @@
         <v>141</v>
       </c>
       <c r="J19" s="126" t="str">
-        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
       <c r="K19" s="126" t="str">
-        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L19" s="117"/>
-      <c r="M19" s="117"/>
+      <c r="L19" s="342" t="str">
+        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M19" s="343" t="str">
+        <f>VLOOKUP(I19,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Invitable Participant</v>
+      </c>
       <c r="N19" s="117"/>
       <c r="O19" s="117"/>
       <c r="P19" s="117"/>
@@ -25381,15 +25583,21 @@
         <v>141</v>
       </c>
       <c r="J20" s="126" t="str">
-        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
       <c r="K20" s="126" t="str">
-        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L20" s="117"/>
-      <c r="M20" s="117"/>
+      <c r="L20" s="342" t="str">
+        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M20" s="343" t="str">
+        <f>VLOOKUP(I20,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Invitable Participant</v>
+      </c>
       <c r="N20" s="117"/>
       <c r="O20" s="117"/>
       <c r="P20" s="117"/>
@@ -25474,15 +25682,21 @@
         <v>141</v>
       </c>
       <c r="J21" s="126" t="str">
-        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
       <c r="K21" s="126" t="str">
-        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L21" s="117"/>
-      <c r="M21" s="117"/>
+      <c r="L21" s="342" t="str">
+        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M21" s="343" t="str">
+        <f>VLOOKUP(I21,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Invitable Participant</v>
+      </c>
       <c r="N21" s="117"/>
       <c r="O21" s="117"/>
       <c r="P21" s="117"/>
@@ -25567,15 +25781,21 @@
         <v>141</v>
       </c>
       <c r="J22" s="126" t="str">
-        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Cohort Manager is concerned with the definition of due participants. Is recieves the eligible cohort from Cohorting As a Service and allows the management of due participants, both in terms of data quality and editing the cohort. It enables the management of external referrals into the screening programme (self or GP).</v>
       </c>
       <c r="K22" s="126" t="str">
-        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Staff users, Secondary users</v>
       </c>
-      <c r="L22" s="117"/>
-      <c r="M22" s="117"/>
+      <c r="L22" s="342" t="str">
+        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M22" s="343" t="str">
+        <f>VLOOKUP(I22,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Invitable Participant</v>
+      </c>
       <c r="N22" s="117"/>
       <c r="O22" s="117"/>
       <c r="P22" s="117"/>
@@ -25660,15 +25880,21 @@
         <v>105</v>
       </c>
       <c r="J23" s="126" t="str">
-        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Allocator is a pathway agnostic allocation engine. It provides a set of allocation algorithms and uses participant preferences and needs e.g. accessibility criteria to optimally allocate individuals to 'slots'.</v>
       </c>
       <c r="K23" s="126" t="str">
-        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>System User</v>
-      </c>
-      <c r="L23" s="117"/>
-      <c r="M23" s="117"/>
+        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Staff users, Secondary users</v>
+      </c>
+      <c r="L23" s="342" t="str">
+        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Allocation</v>
+      </c>
+      <c r="M23" s="343" t="str">
+        <f>VLOOKUP(I23,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Allocation</v>
+      </c>
       <c r="N23" s="117"/>
       <c r="O23" s="117"/>
       <c r="P23" s="117"/>
@@ -25753,15 +25979,21 @@
         <v>105</v>
       </c>
       <c r="J24" s="126" t="str">
-        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Allocator is a pathway agnostic allocation engine. It provides a set of allocation algorithms and uses participant preferences and needs e.g. accessibility criteria to optimally allocate individuals to 'slots'.</v>
       </c>
       <c r="K24" s="126" t="str">
-        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>System User</v>
-      </c>
-      <c r="L24" s="117"/>
-      <c r="M24" s="117"/>
+        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Staff users, Secondary users</v>
+      </c>
+      <c r="L24" s="342" t="str">
+        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Allocation</v>
+      </c>
+      <c r="M24" s="343" t="str">
+        <f>VLOOKUP(I24,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Allocation</v>
+      </c>
       <c r="N24" s="117"/>
       <c r="O24" s="117"/>
       <c r="P24" s="117"/>
@@ -25846,15 +26078,21 @@
         <v>110</v>
       </c>
       <c r="J25" s="126" t="str">
-        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K25" s="126" t="str">
-        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L25" s="117"/>
-      <c r="M25" s="117"/>
+        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L25" s="342" t="str">
+        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M25" s="343" t="str">
+        <f>VLOOKUP(I25,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N25" s="117"/>
       <c r="O25" s="117"/>
       <c r="P25" s="117"/>
@@ -25939,15 +26177,21 @@
         <v>110</v>
       </c>
       <c r="J26" s="126" t="str">
-        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K26" s="126" t="str">
-        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L26" s="117"/>
-      <c r="M26" s="117"/>
+        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L26" s="342" t="str">
+        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M26" s="343" t="str">
+        <f>VLOOKUP(I26,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N26" s="117"/>
       <c r="O26" s="117"/>
       <c r="P26" s="117"/>
@@ -26032,15 +26276,21 @@
         <v>110</v>
       </c>
       <c r="J27" s="126" t="str">
-        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K27" s="126" t="str">
-        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L27" s="117"/>
-      <c r="M27" s="117"/>
+        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L27" s="342" t="str">
+        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M27" s="343" t="str">
+        <f>VLOOKUP(I27,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N27" s="117"/>
       <c r="O27" s="117"/>
       <c r="P27" s="117"/>
@@ -26125,15 +26375,21 @@
         <v>110</v>
       </c>
       <c r="J28" s="126" t="str">
-        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K28" s="126" t="str">
-        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L28" s="117"/>
-      <c r="M28" s="117"/>
+        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L28" s="342" t="str">
+        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M28" s="343" t="str">
+        <f>VLOOKUP(I28,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N28" s="117"/>
       <c r="O28" s="117"/>
       <c r="P28" s="117"/>
@@ -26218,15 +26474,21 @@
         <v>216</v>
       </c>
       <c r="J29" s="126" t="str">
-        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
       <c r="K29" s="126" t="str">
-        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L29" s="117"/>
-      <c r="M29" s="117"/>
+      <c r="L29" s="342" t="str">
+        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Communication</v>
+      </c>
+      <c r="M29" s="343" t="str">
+        <f>VLOOKUP(I29,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Letter, Email, Text Message</v>
+      </c>
       <c r="N29" s="117"/>
       <c r="O29" s="117"/>
       <c r="P29" s="117"/>
@@ -26311,15 +26573,21 @@
         <v>157</v>
       </c>
       <c r="J30" s="126" t="str">
-        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K30" s="126" t="str">
-        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L30" s="117"/>
-      <c r="M30" s="117"/>
+      <c r="L30" s="342" t="str">
+        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M30" s="343" t="str">
+        <f>VLOOKUP(I30,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N30" s="117"/>
       <c r="O30" s="117"/>
       <c r="P30" s="117"/>
@@ -26404,15 +26672,21 @@
         <v>157</v>
       </c>
       <c r="J31" s="126" t="str">
-        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K31" s="126" t="str">
-        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L31" s="117"/>
-      <c r="M31" s="117"/>
+      <c r="L31" s="342" t="str">
+        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M31" s="343" t="str">
+        <f>VLOOKUP(I31,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N31" s="117"/>
       <c r="O31" s="117"/>
       <c r="P31" s="117"/>
@@ -26497,15 +26771,21 @@
         <v>157</v>
       </c>
       <c r="J32" s="126" t="str">
-        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K32" s="126" t="str">
-        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L32" s="117"/>
-      <c r="M32" s="117"/>
+      <c r="L32" s="342" t="str">
+        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M32" s="343" t="str">
+        <f>VLOOKUP(I32,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N32" s="117"/>
       <c r="O32" s="117"/>
       <c r="P32" s="117"/>
@@ -26590,15 +26870,21 @@
         <v>157</v>
       </c>
       <c r="J33" s="126" t="str">
-        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K33" s="126" t="str">
-        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L33" s="117"/>
-      <c r="M33" s="117"/>
+      <c r="L33" s="342" t="str">
+        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M33" s="343" t="str">
+        <f>VLOOKUP(I33,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N33" s="117"/>
       <c r="O33" s="117"/>
       <c r="P33" s="117"/>
@@ -26683,15 +26969,21 @@
         <v>216</v>
       </c>
       <c r="J34" s="126" t="str">
-        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
       <c r="K34" s="126" t="str">
-        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L34" s="117"/>
-      <c r="M34" s="117"/>
+      <c r="L34" s="342" t="str">
+        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Communication</v>
+      </c>
+      <c r="M34" s="343" t="str">
+        <f>VLOOKUP(I34,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Letter, Email, Text Message</v>
+      </c>
       <c r="N34" s="117"/>
       <c r="O34" s="117"/>
       <c r="P34" s="117"/>
@@ -26776,15 +27068,21 @@
         <v>216</v>
       </c>
       <c r="J35" s="126" t="str">
-        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
       <c r="K35" s="126" t="str">
-        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L35" s="117"/>
-      <c r="M35" s="117"/>
+      <c r="L35" s="342" t="str">
+        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Communication</v>
+      </c>
+      <c r="M35" s="343" t="str">
+        <f>VLOOKUP(I35,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Letter, Email, Text Message</v>
+      </c>
       <c r="N35" s="117"/>
       <c r="O35" s="117"/>
       <c r="P35" s="117"/>
@@ -26869,15 +27167,21 @@
         <v>110</v>
       </c>
       <c r="J36" s="126" t="str">
-        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K36" s="126" t="str">
-        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L36" s="117"/>
-      <c r="M36" s="117"/>
+        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L36" s="342" t="str">
+        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M36" s="343" t="str">
+        <f>VLOOKUP(I36,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N36" s="117"/>
       <c r="O36" s="117"/>
       <c r="P36" s="117"/>
@@ -26962,15 +27266,21 @@
         <v>110</v>
       </c>
       <c r="J37" s="126" t="str">
-        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K37" s="126" t="str">
-        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L37" s="117"/>
-      <c r="M37" s="117"/>
+        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L37" s="342" t="str">
+        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M37" s="343" t="str">
+        <f>VLOOKUP(I37,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N37" s="117"/>
       <c r="O37" s="117"/>
       <c r="P37" s="117"/>
@@ -27055,15 +27365,21 @@
         <v>110</v>
       </c>
       <c r="J38" s="126" t="str">
-        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K38" s="126" t="str">
-        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L38" s="117"/>
-      <c r="M38" s="117"/>
+        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L38" s="342" t="str">
+        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M38" s="343" t="str">
+        <f>VLOOKUP(I38,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N38" s="117"/>
       <c r="O38" s="117"/>
       <c r="P38" s="117"/>
@@ -27148,15 +27464,21 @@
         <v>172</v>
       </c>
       <c r="J39" s="126" t="str">
-        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Support allows the efficient handling of inbound queries from participants about the screening pathway and will primarily be used by participant support staff e.g. call centre staff.</v>
       </c>
       <c r="K39" s="126" t="str">
-        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users</v>
       </c>
-      <c r="L39" s="117"/>
-      <c r="M39" s="117"/>
+      <c r="L39" s="342">
+        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="343">
+        <f>VLOOKUP(I39,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>0</v>
+      </c>
       <c r="N39" s="117"/>
       <c r="O39" s="117"/>
       <c r="P39" s="117"/>
@@ -27241,15 +27563,21 @@
         <v>172</v>
       </c>
       <c r="J40" s="126" t="str">
-        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Support allows the efficient handling of inbound queries from participants about the screening pathway and will primarily be used by participant support staff e.g. call centre staff.</v>
       </c>
       <c r="K40" s="126" t="str">
-        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users</v>
       </c>
-      <c r="L40" s="117"/>
-      <c r="M40" s="117"/>
+      <c r="L40" s="342">
+        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="343">
+        <f>VLOOKUP(I40,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>0</v>
+      </c>
       <c r="N40" s="117"/>
       <c r="O40" s="117"/>
       <c r="P40" s="117"/>
@@ -27334,15 +27662,21 @@
         <v>110</v>
       </c>
       <c r="J41" s="126" t="str">
-        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K41" s="126" t="str">
-        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L41" s="117"/>
-      <c r="M41" s="117"/>
+        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L41" s="342" t="str">
+        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M41" s="343" t="str">
+        <f>VLOOKUP(I41,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N41" s="117"/>
       <c r="O41" s="117"/>
       <c r="P41" s="117"/>
@@ -27427,15 +27761,21 @@
         <v>110</v>
       </c>
       <c r="J42" s="126" t="str">
-        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Appointment Booker supports the management of appointments from both the participant and provider perspective. It allows both participants and providers to create, amend and cancel appointments. Providers can manage available slots based on real-time capacity and can ensure that invitations and reminders are triggered at appropriate points in the screening pathway.</v>
       </c>
       <c r="K42" s="126" t="str">
-        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Participant users, Staff users, Secondary users</v>
-      </c>
-      <c r="L42" s="117"/>
-      <c r="M42" s="117"/>
+        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>System User</v>
+      </c>
+      <c r="L42" s="342" t="str">
+        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Appointment</v>
+      </c>
+      <c r="M42" s="343" t="str">
+        <f>VLOOKUP(I42,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Appointment</v>
+      </c>
       <c r="N42" s="117"/>
       <c r="O42" s="117"/>
       <c r="P42" s="117"/>
@@ -27520,15 +27860,21 @@
         <v>157</v>
       </c>
       <c r="J43" s="126" t="str">
-        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K43" s="126" t="str">
-        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L43" s="117"/>
-      <c r="M43" s="117"/>
+      <c r="L43" s="342" t="str">
+        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M43" s="343" t="str">
+        <f>VLOOKUP(I43,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N43" s="117"/>
       <c r="O43" s="117"/>
       <c r="P43" s="117"/>
@@ -27613,15 +27959,21 @@
         <v>157</v>
       </c>
       <c r="J44" s="126" t="str">
-        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K44" s="126" t="str">
-        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L44" s="117"/>
-      <c r="M44" s="117"/>
+      <c r="L44" s="342" t="str">
+        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M44" s="343" t="str">
+        <f>VLOOKUP(I44,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N44" s="117"/>
       <c r="O44" s="117"/>
       <c r="P44" s="117"/>
@@ -27706,15 +28058,21 @@
         <v>157</v>
       </c>
       <c r="J45" s="126" t="str">
-        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Participant Manager manages all screening information about the participant. Participants can view their screening history, self refer, amend appointments and provide data relevant to the screening pathway e.g. accessibility requirements or pre-screening questionnaires. Additionally, Participant Manager enables providers to provide appropriate content to promote uptake, review screening hitsory and assist participants through the screening pathway.</v>
       </c>
       <c r="K45" s="126" t="str">
-        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant users, Staff users, Tertiary users</v>
       </c>
-      <c r="L45" s="117"/>
-      <c r="M45" s="117"/>
+      <c r="L45" s="342" t="str">
+        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Participant</v>
+      </c>
+      <c r="M45" s="343" t="str">
+        <f>VLOOKUP(I45,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Participant, Episode</v>
+      </c>
       <c r="N45" s="117"/>
       <c r="O45" s="117"/>
       <c r="P45" s="117"/>
@@ -27799,15 +28157,21 @@
         <v>186</v>
       </c>
       <c r="J46" s="126" t="str">
-        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K46" s="126" t="str">
-        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L46" s="117"/>
-      <c r="M46" s="117"/>
+      <c r="L46" s="342" t="str">
+        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M46" s="343" t="str">
+        <f>VLOOKUP(I46,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N46" s="117"/>
       <c r="O46" s="117"/>
       <c r="P46" s="117"/>
@@ -27892,15 +28256,21 @@
         <v>186</v>
       </c>
       <c r="J47" s="126" t="str">
-        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K47" s="126" t="str">
-        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L47" s="117"/>
-      <c r="M47" s="117"/>
+      <c r="L47" s="342" t="str">
+        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M47" s="343" t="str">
+        <f>VLOOKUP(I47,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N47" s="117"/>
       <c r="O47" s="117"/>
       <c r="P47" s="117"/>
@@ -27985,15 +28355,21 @@
         <v>186</v>
       </c>
       <c r="J48" s="126" t="str">
-        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K48" s="126" t="str">
-        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
+      <c r="L48" s="342" t="str">
+        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M48" s="343" t="str">
+        <f>VLOOKUP(I48,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N48" s="117"/>
       <c r="O48" s="117"/>
       <c r="P48" s="117"/>
@@ -28078,15 +28454,21 @@
         <v>186</v>
       </c>
       <c r="J49" s="126" t="str">
-        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K49" s="126" t="str">
-        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L49" s="117"/>
-      <c r="M49" s="117"/>
+      <c r="L49" s="342" t="str">
+        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M49" s="343" t="str">
+        <f>VLOOKUP(I49,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N49" s="117"/>
       <c r="O49" s="117"/>
       <c r="P49" s="117"/>
@@ -28171,15 +28553,21 @@
         <v>186</v>
       </c>
       <c r="J50" s="126" t="str">
-        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K50" s="126" t="str">
-        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L50" s="117"/>
-      <c r="M50" s="117"/>
+      <c r="L50" s="342" t="str">
+        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M50" s="343" t="str">
+        <f>VLOOKUP(I50,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N50" s="117"/>
       <c r="O50" s="117"/>
       <c r="P50" s="117"/>
@@ -28264,15 +28652,21 @@
         <v>186</v>
       </c>
       <c r="J51" s="126" t="str">
-        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K51" s="126" t="str">
-        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L51" s="117"/>
-      <c r="M51" s="117"/>
+      <c r="L51" s="342" t="str">
+        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M51" s="343" t="str">
+        <f>VLOOKUP(I51,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N51" s="117"/>
       <c r="O51" s="117"/>
       <c r="P51" s="117"/>
@@ -28357,15 +28751,21 @@
         <v>186</v>
       </c>
       <c r="J52" s="126" t="str">
-        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Screening Event Manager coordinates the clinical aspect of the screening pathway e.g. the clinical investigation, sample analysis and ultimate diagnosis. It provides the ability to capture data as the participant flows through the clinical portion of the screening pathway.</v>
       </c>
       <c r="K52" s="126" t="str">
-        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Participant, Staff users, Tertiary users</v>
       </c>
-      <c r="L52" s="117"/>
-      <c r="M52" s="117"/>
+      <c r="L52" s="342" t="str">
+        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Clinical, Diagnostic</v>
+      </c>
+      <c r="M52" s="343" t="str">
+        <f>VLOOKUP(I52,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Sample, Clinical Analysis, Findings, Diagnosis, Outcomes</v>
+      </c>
       <c r="N52" s="117"/>
       <c r="O52" s="117"/>
       <c r="P52" s="117"/>
@@ -28450,15 +28850,21 @@
         <v>175</v>
       </c>
       <c r="J53" s="126" t="str">
-        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K53" s="126" t="str">
-        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L53" s="117"/>
-      <c r="M53" s="117"/>
+      <c r="L53" s="342" t="str">
+        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M53" s="343" t="str">
+        <f>VLOOKUP(I53,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N53" s="117"/>
       <c r="O53" s="117"/>
       <c r="P53" s="117"/>
@@ -28543,15 +28949,21 @@
         <v>175</v>
       </c>
       <c r="J54" s="126" t="str">
-        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K54" s="126" t="str">
-        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L54" s="117"/>
-      <c r="M54" s="117"/>
+      <c r="L54" s="342" t="str">
+        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M54" s="343" t="str">
+        <f>VLOOKUP(I54,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N54" s="117"/>
       <c r="O54" s="117"/>
       <c r="P54" s="117"/>
@@ -28636,15 +29048,21 @@
         <v>175</v>
       </c>
       <c r="J55" s="126" t="str">
-        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K55" s="126" t="str">
-        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L55" s="117"/>
-      <c r="M55" s="117"/>
+      <c r="L55" s="342" t="str">
+        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M55" s="343" t="str">
+        <f>VLOOKUP(I55,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N55" s="117"/>
       <c r="O55" s="117"/>
       <c r="P55" s="117"/>
@@ -28729,15 +29147,21 @@
         <v>175</v>
       </c>
       <c r="J56" s="126" t="str">
-        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K56" s="126" t="str">
-        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L56" s="117"/>
-      <c r="M56" s="117"/>
+      <c r="L56" s="342" t="str">
+        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M56" s="343" t="str">
+        <f>VLOOKUP(I56,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N56" s="117"/>
       <c r="O56" s="117"/>
       <c r="P56" s="117"/>
@@ -28822,15 +29246,21 @@
         <v>216</v>
       </c>
       <c r="J57" s="126" t="str">
-        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">Communications Manager acts as a common way of communcating with participants by leveraging NHS Notify. It enables personalised communication, with differerent templates applied according to the specific scenario and accounts for participant communication preferences. </v>
       </c>
       <c r="K57" s="126" t="str">
-        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L57" s="117"/>
-      <c r="M57" s="117"/>
+      <c r="L57" s="342" t="str">
+        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Communication</v>
+      </c>
+      <c r="M57" s="343" t="str">
+        <f>VLOOKUP(I57,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Letter, Email, Text Message</v>
+      </c>
       <c r="N57" s="117"/>
       <c r="O57" s="117"/>
       <c r="P57" s="117"/>
@@ -28915,15 +29345,21 @@
         <v>87</v>
       </c>
       <c r="J58" s="126" t="str">
-        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K58" s="126" t="str">
-        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L58" s="117"/>
-      <c r="M58" s="117"/>
+        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L58" s="342" t="str">
+        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M58" s="343" t="str">
+        <f>VLOOKUP(I58,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N58" s="117"/>
       <c r="O58" s="117"/>
       <c r="P58" s="117"/>
@@ -29008,15 +29444,21 @@
         <v>175</v>
       </c>
       <c r="J59" s="126" t="str">
-        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Pathway Coordinator is the engine of the screening pathway. It allows core elements of screening pathways to be updated e.g. eligibilty criteria or screening intervals. Pathway Coordinator fulfills the pathway for each participant by managing data flow between products according to each specific pathway's definition. Pathway coordinator manages the screening outcome, including updating a participant's future pathway allocation and communicating to external sources e.g. GP and other healthcare professionals involved in treatment pathways.</v>
       </c>
       <c r="K59" s="126" t="str">
-        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L59" s="117"/>
-      <c r="M59" s="117"/>
+      <c r="L59" s="342" t="str">
+        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Pathway</v>
+      </c>
+      <c r="M59" s="343" t="str">
+        <f>VLOOKUP(I59,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Requirement for slot, Encounter</v>
+      </c>
       <c r="N59" s="117"/>
       <c r="O59" s="117"/>
       <c r="P59" s="117"/>
@@ -29101,15 +29543,21 @@
         <v>87</v>
       </c>
       <c r="J60" s="126" t="str">
-        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K60" s="126" t="str">
-        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L60" s="117"/>
-      <c r="M60" s="117"/>
+        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L60" s="342" t="str">
+        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M60" s="343" t="str">
+        <f>VLOOKUP(I60,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N60" s="117"/>
       <c r="O60" s="117"/>
       <c r="P60" s="117"/>
@@ -29194,15 +29642,21 @@
         <v>87</v>
       </c>
       <c r="J61" s="126" t="str">
-        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K61" s="126" t="str">
-        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L61" s="117"/>
-      <c r="M61" s="117"/>
+        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L61" s="342" t="str">
+        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M61" s="343" t="str">
+        <f>VLOOKUP(I61,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N61" s="117"/>
       <c r="O61" s="117"/>
       <c r="P61" s="117"/>
@@ -29287,15 +29741,21 @@
         <v>87</v>
       </c>
       <c r="J62" s="126" t="str">
-        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K62" s="126" t="str">
-        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L62" s="117"/>
-      <c r="M62" s="117"/>
+        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L62" s="342" t="str">
+        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M62" s="343" t="str">
+        <f>VLOOKUP(I62,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N62" s="117"/>
       <c r="O62" s="117"/>
       <c r="P62" s="117"/>
@@ -29380,15 +29840,21 @@
         <v>122</v>
       </c>
       <c r="J63" s="126" t="str">
-        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v>Business Audit captures all events that occur for a participant across a screening pathway e.g. digital communications, appointment attendance. It does this in a manner that prevents data tampering and is used for  non repudiation, clinical safety and identification and investigation of incidents.</v>
       </c>
       <c r="K63" s="126" t="str">
-        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
+        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
         <v>Secondary users</v>
       </c>
-      <c r="L63" s="117"/>
-      <c r="M63" s="117"/>
+      <c r="L63" s="342" t="str">
+        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>Audit</v>
+      </c>
+      <c r="M63" s="343" t="str">
+        <f>VLOOKUP(I63,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>Audit</v>
+      </c>
       <c r="N63" s="117"/>
       <c r="O63" s="117"/>
       <c r="P63" s="117"/>
@@ -29473,15 +29939,21 @@
         <v>87</v>
       </c>
       <c r="J64" s="126" t="str">
-        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K64" s="126" t="str">
-        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L64" s="117"/>
-      <c r="M64" s="117"/>
+        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L64" s="342" t="str">
+        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M64" s="343" t="str">
+        <f>VLOOKUP(I64,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N64" s="117"/>
       <c r="O64" s="117"/>
       <c r="P64" s="117"/>
@@ -29566,15 +30038,21 @@
         <v>87</v>
       </c>
       <c r="J65" s="126" t="str">
-        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$B$14,2,FALSE)</f>
+        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$B$15,2,FALSE)</f>
         <v xml:space="preserve">BI and Data Analysis facilitates data-driven decisions to optimise screening pathways. It enables a variety of users, ranging from programme managers, to quality assurance and researchers to interrogate screening data. By joining together different datasets, it allows users to segment participants according to different attributes e.g. clinical risk factors or participant behaviour and to review provider performance at different levels of granularity. </v>
       </c>
       <c r="K65" s="126" t="str">
-        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$C$14,3,FALSE)</f>
-        <v>Staff users, Secondary users</v>
-      </c>
-      <c r="L65" s="117"/>
-      <c r="M65" s="117"/>
+        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$C$15,3,FALSE)</f>
+        <v>Participant users, Staff users, Secondary users</v>
+      </c>
+      <c r="L65" s="342" t="str">
+        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$E$18,4,FALSE)</f>
+        <v>n/a</v>
+      </c>
+      <c r="M65" s="343" t="str">
+        <f>VLOOKUP(I65,'Product Definitions'!$A$2:$E$18,5,FALSE)</f>
+        <v>n/a</v>
+      </c>
       <c r="N65" s="117"/>
       <c r="O65" s="117"/>
       <c r="P65" s="117"/>
@@ -29642,8 +30120,7 @@
       <c r="I66" s="127"/>
       <c r="J66" s="117"/>
       <c r="K66" s="117"/>
-      <c r="L66" s="117"/>
-      <c r="M66" s="117"/>
+      <c r="M66" s="344"/>
       <c r="N66" s="117"/>
       <c r="O66" s="117"/>
       <c r="P66" s="117"/>
@@ -29711,8 +30188,7 @@
       <c r="I67" s="127"/>
       <c r="J67" s="117"/>
       <c r="K67" s="117"/>
-      <c r="L67" s="117"/>
-      <c r="M67" s="117"/>
+      <c r="M67" s="344"/>
       <c r="N67" s="117"/>
       <c r="O67" s="117"/>
       <c r="P67" s="117"/>
@@ -29780,8 +30256,7 @@
       <c r="I68" s="127"/>
       <c r="J68" s="117"/>
       <c r="K68" s="117"/>
-      <c r="L68" s="117"/>
-      <c r="M68" s="117"/>
+      <c r="M68" s="344"/>
       <c r="N68" s="117"/>
       <c r="O68" s="117"/>
       <c r="P68" s="117"/>
@@ -29849,8 +30324,7 @@
       <c r="I69" s="127"/>
       <c r="J69" s="117"/>
       <c r="K69" s="117"/>
-      <c r="L69" s="117"/>
-      <c r="M69" s="117"/>
+      <c r="M69" s="344"/>
       <c r="N69" s="117"/>
       <c r="O69" s="117"/>
       <c r="P69" s="117"/>
@@ -29918,8 +30392,7 @@
       <c r="I70" s="127"/>
       <c r="J70" s="117"/>
       <c r="K70" s="117"/>
-      <c r="L70" s="117"/>
-      <c r="M70" s="117"/>
+      <c r="M70" s="344"/>
       <c r="N70" s="117"/>
       <c r="O70" s="117"/>
       <c r="P70" s="117"/>
@@ -29988,64 +30461,90 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8096783-64B1-C547-94F3-04D3BE1EF5B1}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.33203125" customWidth="1"/>
-    <col min="3" max="3" width="36.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="98" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="337" t="s">
+      <c r="C1" s="303" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="339" t="s">
+        <v>483</v>
+      </c>
+      <c r="E1" s="339" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="180" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="B2" s="178" t="s">
-        <v>386</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E2" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="177" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B3" s="178" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>485</v>
+      </c>
+      <c r="E3" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="177" t="s">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B4" s="178" t="s">
-        <v>111</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>486</v>
+      </c>
+      <c r="E4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="183" t="s">
         <v>122</v>
       </c>
@@ -30055,8 +30554,14 @@
       <c r="C5" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="103" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>482</v>
+      </c>
+      <c r="E5" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="103" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="177" t="s">
         <v>126</v>
       </c>
@@ -30066,8 +30571,14 @@
       <c r="C6" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>487</v>
+      </c>
+      <c r="E6" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="177" t="s">
         <v>131</v>
       </c>
@@ -30077,8 +30588,14 @@
       <c r="C7" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="69" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>489</v>
+      </c>
+      <c r="E7" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="177" t="s">
         <v>137</v>
       </c>
@@ -30088,75 +30605,132 @@
       <c r="C8" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>488</v>
+      </c>
+      <c r="E8" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="177" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="178" t="s">
+        <v>492</v>
+      </c>
+      <c r="C9" t="s">
+        <v>493</v>
+      </c>
+      <c r="D9" t="s">
+        <v>490</v>
+      </c>
+      <c r="E9" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="177" t="s">
         <v>141</v>
       </c>
-      <c r="B9" s="178" t="s">
+      <c r="B10" s="178" t="s">
         <v>142</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="179" t="s">
+      <c r="D10" t="s">
+        <v>490</v>
+      </c>
+      <c r="E10" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="179" t="s">
         <v>216</v>
       </c>
-      <c r="B10" s="178" t="s">
+      <c r="B11" s="178" t="s">
         <v>150</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="120" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="177" t="s">
+      <c r="D11" t="s">
+        <v>481</v>
+      </c>
+      <c r="E11" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="120" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="177" t="s">
         <v>157</v>
       </c>
-      <c r="B11" s="178" t="s">
+      <c r="B12" s="178" t="s">
         <v>158</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="52" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="177" t="s">
+      <c r="D12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E12" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="52" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="177" t="s">
         <v>172</v>
       </c>
-      <c r="B12" s="178" t="s">
+      <c r="B13" s="178" t="s">
         <v>173</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="154" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="177" t="s">
+    <row r="14" spans="1:5" ht="154" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="177" t="s">
         <v>175</v>
       </c>
-      <c r="B13" s="178" t="s">
+      <c r="B14" s="178" t="s">
         <v>176</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="86" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="182" t="s">
+      <c r="D14" t="s">
+        <v>494</v>
+      </c>
+      <c r="E14" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="86" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="182" t="s">
         <v>186</v>
       </c>
-      <c r="B14" s="181" t="s">
+      <c r="B15" s="181" t="s">
         <v>187</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>396</v>
       </c>
+      <c r="D15" t="s">
+        <v>495</v>
+      </c>
+      <c r="E15" t="s">
+        <v>504</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{F8096783-64B1-C547-94F3-04D3BE1EF5B1}"/>
+  <autoFilter ref="A1:B1" xr:uid="{F8096783-64B1-C547-94F3-04D3BE1EF5B1}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B14">
+      <sortCondition ref="A1:A14"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -30874,12 +31448,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -31051,15 +31622,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBF2C2CF-D33D-481D-9646-EB696D575B46}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9013F849-835B-4B56-979A-6E3BED8C8116}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="d5a2e99d-d1f9-4394-b555-45eb01e24998"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -31083,17 +31665,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9013F849-835B-4B56-979A-6E3BED8C8116}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBF2C2CF-D33D-481D-9646-EB696D575B46}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="d5a2e99d-d1f9-4394-b555-45eb01e24998"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>